<commit_message>
format output r^2 values
</commit_message>
<xml_diff>
--- a/part2/tables-2/dom_validty_VER_part-2.xlsx
+++ b/part2/tables-2/dom_validty_VER_part-2.xlsx
@@ -426,13 +426,13 @@
         <v>6</v>
       </c>
       <c r="C2">
-        <v>0.00615</v>
+        <v>0.023898</v>
       </c>
       <c r="D2">
-        <v>0.004948</v>
+        <v>0.08387600000000001</v>
       </c>
       <c r="F2">
-        <v>0.195493</v>
+        <v>-2.509709</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -443,13 +443,13 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>0.003149</v>
+        <v>0.012234</v>
       </c>
       <c r="D3">
-        <v>0.001212</v>
+        <v>0.017302</v>
       </c>
       <c r="F3">
-        <v>0.614936</v>
+        <v>-0.414278</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -460,13 +460,13 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>0.001764</v>
+        <v>0.006321</v>
       </c>
       <c r="D4">
-        <v>0.000293</v>
+        <v>0.003263</v>
       </c>
       <c r="F4">
-        <v>0.834035</v>
+        <v>0.48381</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -477,13 +477,13 @@
         <v>6</v>
       </c>
       <c r="C5">
-        <v>0.000891</v>
+        <v>0.003462</v>
       </c>
       <c r="D5">
-        <v>8.000000000000001E-05</v>
+        <v>0.000669</v>
       </c>
       <c r="F5">
-        <v>0.910704</v>
+        <v>0.80676</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -494,13 +494,13 @@
         <v>6</v>
       </c>
       <c r="C6">
-        <v>0.005868</v>
+        <v>0.029379</v>
       </c>
       <c r="D6">
-        <v>0.004173</v>
+        <v>0.065481</v>
       </c>
       <c r="F6">
-        <v>0.288933</v>
+        <v>-1.228827</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -511,13 +511,13 @@
         <v>6</v>
       </c>
       <c r="C7">
-        <v>0.002934</v>
+        <v>0.019388</v>
       </c>
       <c r="D7">
-        <v>0.001062</v>
+        <v>0.015438</v>
       </c>
       <c r="F7">
-        <v>0.638056</v>
+        <v>0.20374</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -528,13 +528,13 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <v>0.002402</v>
+        <v>0.011025</v>
       </c>
       <c r="D8">
-        <v>0.00045</v>
+        <v>0.004843</v>
       </c>
       <c r="F8">
-        <v>0.8124670000000001</v>
+        <v>0.560685</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -545,13 +545,13 @@
         <v>6</v>
       </c>
       <c r="C9">
-        <v>0.00107</v>
+        <v>0.006425</v>
       </c>
       <c r="D9">
-        <v>0.000106</v>
+        <v>0.000964</v>
       </c>
       <c r="F9">
-        <v>0.901201</v>
+        <v>0.849979</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -562,13 +562,13 @@
         <v>6</v>
       </c>
       <c r="C10">
-        <v>0.000602</v>
+        <v>0.003015</v>
       </c>
       <c r="D10">
-        <v>3.7E-05</v>
+        <v>0.000287</v>
       </c>
       <c r="F10">
-        <v>0.937859</v>
+        <v>0.904778</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -579,13 +579,13 @@
         <v>6</v>
       </c>
       <c r="C11">
-        <v>0.002797</v>
+        <v>0.022581</v>
       </c>
       <c r="D11">
-        <v>0.001448</v>
+        <v>0.018846</v>
       </c>
       <c r="F11">
-        <v>0.482432</v>
+        <v>0.16541</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -596,13 +596,13 @@
         <v>6</v>
       </c>
       <c r="C12">
-        <v>0.001691</v>
+        <v>0.013655</v>
       </c>
       <c r="D12">
-        <v>0.000451</v>
+        <v>0.005604</v>
       </c>
       <c r="F12">
-        <v>0.733201</v>
+        <v>0.589615</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -613,13 +613,13 @@
         <v>6</v>
       </c>
       <c r="C13">
-        <v>0.000943</v>
+        <v>0.00761</v>
       </c>
       <c r="D13">
-        <v>0.000143</v>
+        <v>0.001499</v>
       </c>
       <c r="F13">
-        <v>0.848606</v>
+        <v>0.803023</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -630,13 +630,13 @@
         <v>6</v>
       </c>
       <c r="C14">
-        <v>0.000411</v>
+        <v>0.003316</v>
       </c>
       <c r="D14">
-        <v>4.7E-05</v>
+        <v>0.000423</v>
       </c>
       <c r="F14">
-        <v>0.885115</v>
+        <v>0.872564</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -647,13 +647,13 @@
         <v>6</v>
       </c>
       <c r="C15">
-        <v>0.000215</v>
+        <v>0.002149</v>
       </c>
       <c r="D15">
-        <v>2.7E-05</v>
+        <v>0.000248</v>
       </c>
       <c r="F15">
-        <v>0.875372</v>
+        <v>0.884486</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -664,13 +664,13 @@
         <v>6</v>
       </c>
       <c r="C16">
-        <v>0.001588</v>
+        <v>0.015863</v>
       </c>
       <c r="D16">
-        <v>0.000454</v>
+        <v>0.006283</v>
       </c>
       <c r="F16">
-        <v>0.714279</v>
+        <v>0.603896</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -681,13 +681,13 @@
         <v>6</v>
       </c>
       <c r="C17">
-        <v>0.001304</v>
+        <v>0.011696</v>
       </c>
       <c r="D17">
-        <v>0.000177</v>
+        <v>0.001975</v>
       </c>
       <c r="F17">
-        <v>0.86443</v>
+        <v>0.831171</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -698,13 +698,13 @@
         <v>6</v>
       </c>
       <c r="C18">
-        <v>0.000779</v>
+        <v>0.006986</v>
       </c>
       <c r="D18">
-        <v>6.7E-05</v>
+        <v>0.0006489999999999999</v>
       </c>
       <c r="F18">
-        <v>0.914502</v>
+        <v>0.907134</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -715,13 +715,13 @@
         <v>6</v>
       </c>
       <c r="C19">
-        <v>0.000398</v>
+        <v>0.003566</v>
       </c>
       <c r="D19">
-        <v>3.2E-05</v>
+        <v>0.000295</v>
       </c>
       <c r="F19">
-        <v>0.918837</v>
+        <v>0.917281</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -732,13 +732,13 @@
         <v>6</v>
       </c>
       <c r="C20">
-        <v>0.00221</v>
+        <v>0.022074</v>
       </c>
       <c r="D20">
-        <v>0.000612</v>
+        <v>0.007860000000000001</v>
       </c>
       <c r="F20">
-        <v>0.723221</v>
+        <v>0.643935</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -749,13 +749,13 @@
         <v>6</v>
       </c>
       <c r="C21">
-        <v>0.001128</v>
+        <v>0.012619</v>
       </c>
       <c r="D21">
-        <v>0.000224</v>
+        <v>0.002809</v>
       </c>
       <c r="F21">
-        <v>0.801214</v>
+        <v>0.77737</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -766,13 +766,13 @@
         <v>6</v>
       </c>
       <c r="C22">
-        <v>0.00072</v>
+        <v>0.008056000000000001</v>
       </c>
       <c r="D22">
-        <v>9.1E-05</v>
+        <v>0.001013</v>
       </c>
       <c r="F22">
-        <v>0.873078</v>
+        <v>0.874245</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -783,13 +783,13 @@
         <v>6</v>
       </c>
       <c r="C23">
-        <v>0.000378</v>
+        <v>0.004231</v>
       </c>
       <c r="D23">
-        <v>4.2E-05</v>
+        <v>0.000423</v>
       </c>
       <c r="F23">
-        <v>0.889852</v>
+        <v>0.900037</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -800,13 +800,13 @@
         <v>6</v>
       </c>
       <c r="C24">
-        <v>0.001462</v>
+        <v>0.023636</v>
       </c>
       <c r="D24">
-        <v>0.000624</v>
+        <v>0.010492</v>
       </c>
       <c r="F24">
-        <v>0.573472</v>
+        <v>0.5560850000000001</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -817,13 +817,13 @@
         <v>6</v>
       </c>
       <c r="C25">
-        <v>0.001034</v>
+        <v>0.016717</v>
       </c>
       <c r="D25">
-        <v>0.000291</v>
+        <v>0.004479</v>
       </c>
       <c r="F25">
-        <v>0.718959</v>
+        <v>0.732043</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -834,13 +834,13 @@
         <v>6</v>
       </c>
       <c r="C26">
-        <v>0.000615</v>
+        <v>0.009950000000000001</v>
       </c>
       <c r="D26">
-        <v>0.000137</v>
+        <v>0.001894</v>
       </c>
       <c r="F26">
-        <v>0.777014</v>
+        <v>0.809602</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -851,13 +851,13 @@
         <v>6</v>
       </c>
       <c r="C27">
-        <v>0.000329</v>
+        <v>0.005314</v>
       </c>
       <c r="D27">
-        <v>6.4E-05</v>
+        <v>0.000791</v>
       </c>
       <c r="F27">
-        <v>0.805608</v>
+        <v>0.851108</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -868,13 +868,13 @@
         <v>6</v>
       </c>
       <c r="C28">
-        <v>0.006257</v>
+        <v>0.024311</v>
       </c>
       <c r="D28">
-        <v>0.004948</v>
+        <v>0.08387600000000001</v>
       </c>
       <c r="F28">
-        <v>0.209144</v>
+        <v>-2.450156</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -885,13 +885,13 @@
         <v>6</v>
       </c>
       <c r="C29">
-        <v>0.003363</v>
+        <v>0.013068</v>
       </c>
       <c r="D29">
-        <v>0.001212</v>
+        <v>0.017302</v>
       </c>
       <c r="F29">
-        <v>0.639514</v>
+        <v>-0.324005</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -902,13 +902,13 @@
         <v>6</v>
       </c>
       <c r="C30">
-        <v>0.001676</v>
+        <v>0.006005</v>
       </c>
       <c r="D30">
-        <v>0.000293</v>
+        <v>0.003263</v>
       </c>
       <c r="F30">
-        <v>0.8253</v>
+        <v>0.456643</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -919,13 +919,13 @@
         <v>6</v>
       </c>
       <c r="C31">
-        <v>0.000884</v>
+        <v>0.003434</v>
       </c>
       <c r="D31">
-        <v>8.000000000000001E-05</v>
+        <v>0.000669</v>
       </c>
       <c r="F31">
-        <v>0.9099660000000001</v>
+        <v>0.805163</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -936,13 +936,13 @@
         <v>6</v>
       </c>
       <c r="C32">
-        <v>0.005729</v>
+        <v>0.02868</v>
       </c>
       <c r="D32">
-        <v>0.004173</v>
+        <v>0.065481</v>
       </c>
       <c r="F32">
-        <v>0.271589</v>
+        <v>-1.283191</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -953,13 +953,13 @@
         <v>6</v>
       </c>
       <c r="C33">
-        <v>0.002923</v>
+        <v>0.019317</v>
       </c>
       <c r="D33">
-        <v>0.001062</v>
+        <v>0.015438</v>
       </c>
       <c r="F33">
-        <v>0.636731</v>
+        <v>0.200824</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -970,13 +970,13 @@
         <v>6</v>
       </c>
       <c r="C34">
-        <v>0.002292</v>
+        <v>0.010519</v>
       </c>
       <c r="D34">
-        <v>0.00045</v>
+        <v>0.004843</v>
       </c>
       <c r="F34">
-        <v>0.803437</v>
+        <v>0.539531</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -987,13 +987,13 @@
         <v>6</v>
       </c>
       <c r="C35">
-        <v>0.000974</v>
+        <v>0.005846</v>
       </c>
       <c r="D35">
-        <v>0.000106</v>
+        <v>0.000964</v>
       </c>
       <c r="F35">
-        <v>0.891416</v>
+        <v>0.835121</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1004,13 +1004,13 @@
         <v>6</v>
       </c>
       <c r="C36">
-        <v>0.000638</v>
+        <v>0.003195</v>
       </c>
       <c r="D36">
-        <v>3.7E-05</v>
+        <v>0.000287</v>
       </c>
       <c r="F36">
-        <v>0.941361</v>
+        <v>0.910145</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1021,13 +1021,13 @@
         <v>6</v>
       </c>
       <c r="C37">
-        <v>0.002806</v>
+        <v>0.022656</v>
       </c>
       <c r="D37">
-        <v>0.001448</v>
+        <v>0.018846</v>
       </c>
       <c r="F37">
-        <v>0.484144</v>
+        <v>0.168171</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1038,13 +1038,13 @@
         <v>6</v>
       </c>
       <c r="C38">
-        <v>0.001712</v>
+        <v>0.013821</v>
       </c>
       <c r="D38">
-        <v>0.000451</v>
+        <v>0.005604</v>
       </c>
       <c r="F38">
-        <v>0.736416</v>
+        <v>0.5945589999999999</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1055,13 +1055,13 @@
         <v>6</v>
       </c>
       <c r="C39">
-        <v>0.000943</v>
+        <v>0.00761</v>
       </c>
       <c r="D39">
-        <v>0.000143</v>
+        <v>0.001499</v>
       </c>
       <c r="F39">
-        <v>0.848606</v>
+        <v>0.803023</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1072,13 +1072,13 @@
         <v>6</v>
       </c>
       <c r="C40">
-        <v>0.000411</v>
+        <v>0.003316</v>
       </c>
       <c r="D40">
-        <v>4.7E-05</v>
+        <v>0.000423</v>
       </c>
       <c r="F40">
-        <v>0.885115</v>
+        <v>0.872564</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1089,13 +1089,13 @@
         <v>6</v>
       </c>
       <c r="C41">
-        <v>0.000219</v>
+        <v>0.002188</v>
       </c>
       <c r="D41">
-        <v>2.7E-05</v>
+        <v>0.000248</v>
       </c>
       <c r="F41">
-        <v>0.877597</v>
+        <v>0.886549</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1106,13 +1106,13 @@
         <v>6</v>
       </c>
       <c r="C42">
-        <v>0.001588</v>
+        <v>0.015863</v>
       </c>
       <c r="D42">
-        <v>0.000454</v>
+        <v>0.006283</v>
       </c>
       <c r="F42">
-        <v>0.714279</v>
+        <v>0.603896</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1123,13 +1123,13 @@
         <v>6</v>
       </c>
       <c r="C43">
-        <v>0.001287</v>
+        <v>0.011538</v>
       </c>
       <c r="D43">
-        <v>0.000177</v>
+        <v>0.001975</v>
       </c>
       <c r="F43">
-        <v>0.862573</v>
+        <v>0.828858</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1140,13 +1140,13 @@
         <v>6</v>
       </c>
       <c r="C44">
-        <v>0.000779</v>
+        <v>0.006986</v>
       </c>
       <c r="D44">
-        <v>6.7E-05</v>
+        <v>0.0006489999999999999</v>
       </c>
       <c r="F44">
-        <v>0.914502</v>
+        <v>0.907134</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1157,13 +1157,13 @@
         <v>6</v>
       </c>
       <c r="C45">
-        <v>0.000377</v>
+        <v>0.003379</v>
       </c>
       <c r="D45">
-        <v>3.2E-05</v>
+        <v>0.000295</v>
       </c>
       <c r="F45">
-        <v>0.914327</v>
+        <v>0.912686</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1174,13 +1174,13 @@
         <v>6</v>
       </c>
       <c r="C46">
-        <v>0.002179</v>
+        <v>0.021766</v>
       </c>
       <c r="D46">
-        <v>0.000612</v>
+        <v>0.007860000000000001</v>
       </c>
       <c r="F46">
-        <v>0.719301</v>
+        <v>0.638891</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1191,13 +1191,13 @@
         <v>6</v>
       </c>
       <c r="C47">
-        <v>0.001195</v>
+        <v>0.013369</v>
       </c>
       <c r="D47">
-        <v>0.000224</v>
+        <v>0.002809</v>
       </c>
       <c r="F47">
-        <v>0.812367</v>
+        <v>0.78986</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1208,13 +1208,13 @@
         <v>6</v>
       </c>
       <c r="C48">
-        <v>0.000695</v>
+        <v>0.007773</v>
       </c>
       <c r="D48">
-        <v>9.1E-05</v>
+        <v>0.001013</v>
       </c>
       <c r="F48">
-        <v>0.868463</v>
+        <v>0.869672</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1225,13 +1225,13 @@
         <v>6</v>
       </c>
       <c r="C49">
-        <v>0.00035</v>
+        <v>0.003918</v>
       </c>
       <c r="D49">
-        <v>4.2E-05</v>
+        <v>0.000423</v>
       </c>
       <c r="F49">
-        <v>0.88104</v>
+        <v>0.8920400000000001</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1242,13 +1242,13 @@
         <v>6</v>
       </c>
       <c r="C50">
-        <v>0.001465</v>
+        <v>0.023686</v>
       </c>
       <c r="D50">
-        <v>0.000624</v>
+        <v>0.010492</v>
       </c>
       <c r="F50">
-        <v>0.57439</v>
+        <v>0.55704</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1259,13 +1259,13 @@
         <v>6</v>
       </c>
       <c r="C51">
-        <v>0.001021</v>
+        <v>0.016512</v>
       </c>
       <c r="D51">
-        <v>0.000291</v>
+        <v>0.004479</v>
       </c>
       <c r="F51">
-        <v>0.7154740000000001</v>
+        <v>0.728721</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -1276,13 +1276,13 @@
         <v>6</v>
       </c>
       <c r="C52">
-        <v>0.000588</v>
+        <v>0.009508000000000001</v>
       </c>
       <c r="D52">
-        <v>0.000137</v>
+        <v>0.001894</v>
       </c>
       <c r="F52">
-        <v>0.766643</v>
+        <v>0.800746</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -1293,13 +1293,13 @@
         <v>6</v>
       </c>
       <c r="C53">
-        <v>0.000313</v>
+        <v>0.005067</v>
       </c>
       <c r="D53">
-        <v>6.4E-05</v>
+        <v>0.000791</v>
       </c>
       <c r="F53">
-        <v>0.796125</v>
+        <v>0.843845</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -1310,13 +1310,13 @@
         <v>6</v>
       </c>
       <c r="C54">
-        <v>0.006915</v>
+        <v>0.026871</v>
       </c>
       <c r="D54">
-        <v>0.006306</v>
+        <v>0.110449</v>
       </c>
       <c r="F54">
-        <v>0.088116</v>
+        <v>-3.110411</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -1327,13 +1327,13 @@
         <v>6</v>
       </c>
       <c r="C55">
-        <v>0.003196</v>
+        <v>0.01242</v>
       </c>
       <c r="D55">
-        <v>0.001575</v>
+        <v>0.02357</v>
       </c>
       <c r="F55">
-        <v>0.507136</v>
+        <v>-0.897742</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -1344,13 +1344,13 @@
         <v>6</v>
       </c>
       <c r="C56">
-        <v>0.001737</v>
+        <v>0.006224</v>
       </c>
       <c r="D56">
-        <v>0.00038</v>
+        <v>0.004465</v>
       </c>
       <c r="F56">
-        <v>0.781213</v>
+        <v>0.282678</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -1361,13 +1361,13 @@
         <v>6</v>
       </c>
       <c r="C57">
-        <v>0.000754</v>
+        <v>0.00293</v>
       </c>
       <c r="D57">
-        <v>9.8E-05</v>
+        <v>0.000857</v>
       </c>
       <c r="F57">
-        <v>0.869689</v>
+        <v>0.7075090000000001</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -1378,13 +1378,13 @@
         <v>6</v>
       </c>
       <c r="C58">
-        <v>0.006604</v>
+        <v>0.033065</v>
       </c>
       <c r="D58">
-        <v>0.005162</v>
+        <v>0.083442</v>
       </c>
       <c r="F58">
-        <v>0.218415</v>
+        <v>-1.523598</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -1395,13 +1395,13 @@
         <v>6</v>
       </c>
       <c r="C59">
-        <v>0.003213</v>
+        <v>0.021233</v>
       </c>
       <c r="D59">
-        <v>0.001311</v>
+        <v>0.019911</v>
       </c>
       <c r="F59">
-        <v>0.59183</v>
+        <v>0.062236</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -1412,13 +1412,13 @@
         <v>6</v>
       </c>
       <c r="C60">
-        <v>0.002574</v>
+        <v>0.011816</v>
       </c>
       <c r="D60">
-        <v>0.000561</v>
+        <v>0.006295</v>
       </c>
       <c r="F60">
-        <v>0.782023</v>
+        <v>0.46724</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -1429,13 +1429,13 @@
         <v>6</v>
       </c>
       <c r="C61">
-        <v>0.001085</v>
+        <v>0.006512</v>
       </c>
       <c r="D61">
-        <v>0.000128</v>
+        <v>0.001214</v>
       </c>
       <c r="F61">
-        <v>0.881818</v>
+        <v>0.813593</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -1446,13 +1446,13 @@
         <v>6</v>
       </c>
       <c r="C62">
-        <v>0.000563</v>
+        <v>0.002817</v>
       </c>
       <c r="D62">
-        <v>4.4E-05</v>
+        <v>0.000338</v>
       </c>
       <c r="F62">
-        <v>0.922647</v>
+        <v>0.8799129999999999</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -1463,13 +1463,13 @@
         <v>6</v>
       </c>
       <c r="C63">
-        <v>0.00299</v>
+        <v>0.024135</v>
       </c>
       <c r="D63">
-        <v>0.001709</v>
+        <v>0.022779</v>
       </c>
       <c r="F63">
-        <v>0.428283</v>
+        <v>0.056193</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -1480,13 +1480,13 @@
         <v>6</v>
       </c>
       <c r="C64">
-        <v>0.001917</v>
+        <v>0.015479</v>
       </c>
       <c r="D64">
-        <v>0.000541</v>
+        <v>0.006966</v>
       </c>
       <c r="F64">
-        <v>0.717803</v>
+        <v>0.549949</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -1497,13 +1497,13 @@
         <v>6</v>
       </c>
       <c r="C65">
-        <v>0.000974</v>
+        <v>0.007865</v>
       </c>
       <c r="D65">
-        <v>0.00017</v>
+        <v>0.00185</v>
       </c>
       <c r="F65">
-        <v>0.825554</v>
+        <v>0.764798</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -1514,13 +1514,13 @@
         <v>6</v>
       </c>
       <c r="C66">
-        <v>0.000448</v>
+        <v>0.003617</v>
       </c>
       <c r="D66">
-        <v>5.4E-05</v>
+        <v>0.000497</v>
       </c>
       <c r="F66">
-        <v>0.878591</v>
+        <v>0.862667</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -1531,13 +1531,13 @@
         <v>6</v>
       </c>
       <c r="C67">
-        <v>0.000244</v>
+        <v>0.00244</v>
       </c>
       <c r="D67">
-        <v>2.9E-05</v>
+        <v>0.000274</v>
       </c>
       <c r="F67">
-        <v>0.879869</v>
+        <v>0.887834</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -1548,13 +1548,13 @@
         <v>6</v>
       </c>
       <c r="C68">
-        <v>0.001829</v>
+        <v>0.018273</v>
       </c>
       <c r="D68">
-        <v>0.000538</v>
+        <v>0.007723</v>
       </c>
       <c r="F68">
-        <v>0.705782</v>
+        <v>0.577353</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -1565,13 +1565,13 @@
         <v>6</v>
       </c>
       <c r="C69">
-        <v>0.001374</v>
+        <v>0.012323</v>
       </c>
       <c r="D69">
-        <v>0.000209</v>
+        <v>0.002409</v>
       </c>
       <c r="F69">
-        <v>0.848149</v>
+        <v>0.804536</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -1582,13 +1582,13 @@
         <v>6</v>
       </c>
       <c r="C70">
-        <v>0.00087</v>
+        <v>0.007802</v>
       </c>
       <c r="D70">
-        <v>7.7E-05</v>
+        <v>0.0007649999999999999</v>
       </c>
       <c r="F70">
-        <v>0.9117960000000001</v>
+        <v>0.901999</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -1599,13 +1599,13 @@
         <v>6</v>
       </c>
       <c r="C71">
-        <v>0.000482</v>
+        <v>0.004322</v>
       </c>
       <c r="D71">
-        <v>3.6E-05</v>
+        <v>0.000329</v>
       </c>
       <c r="F71">
-        <v>0.925908</v>
+        <v>0.923833</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -1616,13 +1616,13 @@
         <v>6</v>
       </c>
       <c r="C72">
-        <v>0.002401</v>
+        <v>0.023986</v>
       </c>
       <c r="D72">
-        <v>0.000713</v>
+        <v>0.009398999999999999</v>
       </c>
       <c r="F72">
-        <v>0.702909</v>
+        <v>0.608127</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -1633,13 +1633,13 @@
         <v>6</v>
       </c>
       <c r="C73">
-        <v>0.001371</v>
+        <v>0.01534</v>
       </c>
       <c r="D73">
-        <v>0.000261</v>
+        <v>0.003362</v>
       </c>
       <c r="F73">
-        <v>0.809984</v>
+        <v>0.780818</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -1650,13 +1650,13 @@
         <v>6</v>
       </c>
       <c r="C74">
-        <v>0.000838</v>
+        <v>0.009372</v>
       </c>
       <c r="D74">
-        <v>0.000105</v>
+        <v>0.001188</v>
       </c>
       <c r="F74">
-        <v>0.875187</v>
+        <v>0.873289</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -1667,13 +1667,13 @@
         <v>6</v>
       </c>
       <c r="C75">
-        <v>0.000439</v>
+        <v>0.004913</v>
       </c>
       <c r="D75">
-        <v>4.6E-05</v>
+        <v>0.000475</v>
       </c>
       <c r="F75">
-        <v>0.894875</v>
+        <v>0.903323</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -1684,13 +1684,13 @@
         <v>6</v>
       </c>
       <c r="C76">
-        <v>0.001639</v>
+        <v>0.026495</v>
       </c>
       <c r="D76">
-        <v>0.000711</v>
+        <v>0.012224</v>
       </c>
       <c r="F76">
-        <v>0.566449</v>
+        <v>0.538642</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -1701,13 +1701,13 @@
         <v>6</v>
       </c>
       <c r="C77">
-        <v>0.001138</v>
+        <v>0.018404</v>
       </c>
       <c r="D77">
-        <v>0.000331</v>
+        <v>0.005235</v>
       </c>
       <c r="F77">
-        <v>0.709351</v>
+        <v>0.71557</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -1718,13 +1718,13 @@
         <v>6</v>
       </c>
       <c r="C78">
-        <v>0.000715</v>
+        <v>0.011565</v>
       </c>
       <c r="D78">
-        <v>0.000155</v>
+        <v>0.002192</v>
       </c>
       <c r="F78">
-        <v>0.783508</v>
+        <v>0.810457</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -1735,13 +1735,13 @@
         <v>6</v>
       </c>
       <c r="C79">
-        <v>0.000405</v>
+        <v>0.00655</v>
       </c>
       <c r="D79">
-        <v>7.1E-05</v>
+        <v>0.000892</v>
       </c>
       <c r="F79">
-        <v>0.825479</v>
+        <v>0.863754</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -1749,13 +1749,13 @@
         <v>79</v>
       </c>
       <c r="C80">
-        <v>0.005957</v>
+        <v>0.023147</v>
       </c>
       <c r="D80">
-        <v>0.005128</v>
+        <v>0.093061</v>
       </c>
       <c r="F80">
-        <v>0.139185</v>
+        <v>-3.020344</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -1766,13 +1766,13 @@
         <v>6</v>
       </c>
       <c r="C81">
-        <v>0.003378</v>
+        <v>0.012102</v>
       </c>
       <c r="D81">
-        <v>0.001322</v>
+        <v>0.019805</v>
       </c>
       <c r="F81">
-        <v>0.6087320000000001</v>
+        <v>-0.636468</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -1783,13 +1783,13 @@
         <v>6</v>
       </c>
       <c r="C82">
-        <v>0.001702</v>
+        <v>0.006614</v>
       </c>
       <c r="D82">
-        <v>0.000289</v>
+        <v>0.003148</v>
       </c>
       <c r="F82">
-        <v>0.830012</v>
+        <v>0.524004</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -1800,13 +1800,13 @@
         <v>6</v>
       </c>
       <c r="C83">
-        <v>0.004729</v>
+        <v>0.031251</v>
       </c>
       <c r="D83">
-        <v>0.003387</v>
+        <v>0.061462</v>
       </c>
       <c r="F83">
-        <v>0.283747</v>
+        <v>-0.966744</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -1814,13 +1814,13 @@
         <v>84</v>
       </c>
       <c r="C84">
-        <v>0.003843</v>
+        <v>0.017637</v>
       </c>
       <c r="D84">
-        <v>0.001559</v>
+        <v>0.021105</v>
       </c>
       <c r="F84">
-        <v>0.594176</v>
+        <v>-0.196659</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -1831,13 +1831,13 @@
         <v>6</v>
       </c>
       <c r="C85">
-        <v>0.001782</v>
+        <v>0.010697</v>
       </c>
       <c r="D85">
-        <v>0.000331</v>
+        <v>0.003875</v>
       </c>
       <c r="F85">
-        <v>0.8141119999999999</v>
+        <v>0.63775</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -1848,13 +1848,13 @@
         <v>6</v>
       </c>
       <c r="C86">
-        <v>0.001185</v>
+        <v>0.005932</v>
       </c>
       <c r="D86">
-        <v>9.7E-05</v>
+        <v>0.000851</v>
       </c>
       <c r="F86">
-        <v>0.917817</v>
+        <v>0.856525</v>
       </c>
     </row>
     <row r="87" spans="1:6">
@@ -1865,13 +1865,13 @@
         <v>6</v>
       </c>
       <c r="C87">
-        <v>0.004203</v>
+        <v>0.03393</v>
       </c>
       <c r="D87">
-        <v>0.003591</v>
+        <v>0.0525</v>
       </c>
       <c r="F87">
-        <v>0.145666</v>
+        <v>-0.547289</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -1882,13 +1882,13 @@
         <v>6</v>
       </c>
       <c r="C88">
-        <v>0.00261</v>
+        <v>0.021071</v>
       </c>
       <c r="D88">
-        <v>0.001246</v>
+        <v>0.018818</v>
       </c>
       <c r="F88">
-        <v>0.522798</v>
+        <v>0.106956</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -1899,13 +1899,13 @@
         <v>6</v>
       </c>
       <c r="C89">
-        <v>0.001491</v>
+        <v>0.012037</v>
       </c>
       <c r="D89">
-        <v>0.000393</v>
+        <v>0.005144</v>
       </c>
       <c r="F89">
-        <v>0.736224</v>
+        <v>0.5726830000000001</v>
       </c>
     </row>
     <row r="90" spans="1:6">
@@ -1916,13 +1916,13 @@
         <v>6</v>
       </c>
       <c r="C90">
-        <v>0.000821</v>
+        <v>0.006625</v>
       </c>
       <c r="D90">
-        <v>0.000114</v>
+        <v>0.001193</v>
       </c>
       <c r="F90">
-        <v>0.860807</v>
+        <v>0.819873</v>
       </c>
     </row>
     <row r="91" spans="1:6">
@@ -1933,13 +1933,13 @@
         <v>6</v>
       </c>
       <c r="C91">
-        <v>0.000418</v>
+        <v>0.004173</v>
       </c>
       <c r="D91">
-        <v>4.9E-05</v>
+        <v>0.00049</v>
       </c>
       <c r="F91">
-        <v>0.8821290000000001</v>
+        <v>0.88269</v>
       </c>
     </row>
     <row r="92" spans="1:6">
@@ -1950,13 +1950,13 @@
         <v>6</v>
       </c>
       <c r="C92">
-        <v>0.002822</v>
+        <v>0.028196</v>
       </c>
       <c r="D92">
-        <v>0.001177</v>
+        <v>0.019747</v>
       </c>
       <c r="F92">
-        <v>0.5829530000000001</v>
+        <v>0.299649</v>
       </c>
     </row>
     <row r="93" spans="1:6">
@@ -1967,13 +1967,13 @@
         <v>6</v>
       </c>
       <c r="C93">
-        <v>0.001907</v>
+        <v>0.017105</v>
       </c>
       <c r="D93">
-        <v>0.000458</v>
+        <v>0.006227</v>
       </c>
       <c r="F93">
-        <v>0.759837</v>
+        <v>0.635961</v>
       </c>
     </row>
     <row r="94" spans="1:6">
@@ -1984,13 +1984,13 @@
         <v>6</v>
       </c>
       <c r="C94">
-        <v>0.0012</v>
+        <v>0.01076</v>
       </c>
       <c r="D94">
-        <v>0.000157</v>
+        <v>0.001785</v>
       </c>
       <c r="F94">
-        <v>0.869507</v>
+        <v>0.834066</v>
       </c>
     </row>
     <row r="95" spans="1:6">
@@ -2001,13 +2001,13 @@
         <v>6</v>
       </c>
       <c r="C95">
-        <v>0.000627</v>
+        <v>0.005626</v>
       </c>
       <c r="D95">
-        <v>6.2E-05</v>
+        <v>0.000613</v>
       </c>
       <c r="F95">
-        <v>0.90111</v>
+        <v>0.890999</v>
       </c>
     </row>
     <row r="96" spans="1:6">
@@ -2018,13 +2018,13 @@
         <v>6</v>
       </c>
       <c r="C96">
-        <v>0.002857</v>
+        <v>0.028537</v>
       </c>
       <c r="D96">
-        <v>0.001437</v>
+        <v>0.021048</v>
       </c>
       <c r="F96">
-        <v>0.497007</v>
+        <v>0.262451</v>
       </c>
     </row>
     <row r="97" spans="1:6">
@@ -2035,13 +2035,13 @@
         <v>6</v>
       </c>
       <c r="C97">
-        <v>0.001794</v>
+        <v>0.020075</v>
       </c>
       <c r="D97">
-        <v>0.000527</v>
+        <v>0.007811</v>
       </c>
       <c r="F97">
-        <v>0.706487</v>
+        <v>0.610895</v>
       </c>
     </row>
     <row r="98" spans="1:6">
@@ -2052,13 +2052,13 @@
         <v>6</v>
       </c>
       <c r="C98">
-        <v>0.001136</v>
+        <v>0.012707</v>
       </c>
       <c r="D98">
-        <v>0.000203</v>
+        <v>0.002624</v>
       </c>
       <c r="F98">
-        <v>0.821661</v>
+        <v>0.793531</v>
       </c>
     </row>
     <row r="99" spans="1:6">
@@ -2069,13 +2069,13 @@
         <v>6</v>
       </c>
       <c r="C99">
-        <v>0.000606</v>
+        <v>0.006784</v>
       </c>
       <c r="D99">
-        <v>8.000000000000001E-05</v>
+        <v>0.000894</v>
       </c>
       <c r="F99">
-        <v>0.868752</v>
+        <v>0.868291</v>
       </c>
     </row>
     <row r="100" spans="1:6">
@@ -2086,13 +2086,13 @@
         <v>6</v>
       </c>
       <c r="C100">
-        <v>0.001978</v>
+        <v>0.031981</v>
       </c>
       <c r="D100">
-        <v>0.001286</v>
+        <v>0.024237</v>
       </c>
       <c r="F100">
-        <v>0.350144</v>
+        <v>0.242164</v>
       </c>
     </row>
     <row r="101" spans="1:6">
@@ -2103,13 +2103,13 @@
         <v>6</v>
       </c>
       <c r="C101">
-        <v>0.001435</v>
+        <v>0.023206</v>
       </c>
       <c r="D101">
-        <v>0.000604</v>
+        <v>0.010733</v>
       </c>
       <c r="F101">
-        <v>0.57931</v>
+        <v>0.537498</v>
       </c>
     </row>
     <row r="102" spans="1:6">
@@ -2120,13 +2120,13 @@
         <v>6</v>
       </c>
       <c r="C102">
-        <v>0.000956</v>
+        <v>0.015462</v>
       </c>
       <c r="D102">
-        <v>0.000276</v>
+        <v>0.00442</v>
       </c>
       <c r="F102">
-        <v>0.711175</v>
+        <v>0.714112</v>
       </c>
     </row>
     <row r="103" spans="1:6">
@@ -2137,13 +2137,13 @@
         <v>6</v>
       </c>
       <c r="C103">
-        <v>0.000535</v>
+        <v>0.008643</v>
       </c>
       <c r="D103">
-        <v>0.000118</v>
+        <v>0.001657</v>
       </c>
       <c r="F103">
-        <v>0.7790550000000001</v>
+        <v>0.808248</v>
       </c>
     </row>
     <row r="104" spans="1:6">
@@ -2154,13 +2154,13 @@
         <v>6</v>
       </c>
       <c r="C104">
-        <v>0.004246</v>
+        <v>0.016497</v>
       </c>
       <c r="D104">
-        <v>0.001637</v>
+        <v>0.023491</v>
       </c>
       <c r="F104">
-        <v>0.6143420000000001</v>
+        <v>-0.424011</v>
       </c>
     </row>
     <row r="105" spans="1:6">
@@ -2171,13 +2171,13 @@
         <v>6</v>
       </c>
       <c r="C105">
-        <v>0.001906</v>
+        <v>0.007407</v>
       </c>
       <c r="D105">
-        <v>0.000387</v>
+        <v>0.004434</v>
       </c>
       <c r="F105">
-        <v>0.7968420000000001</v>
+        <v>0.401381</v>
       </c>
     </row>
     <row r="106" spans="1:6">
@@ -2188,13 +2188,13 @@
         <v>6</v>
       </c>
       <c r="C106">
-        <v>0.001028</v>
+        <v>0.003683</v>
       </c>
       <c r="D106">
-        <v>0.000101</v>
+        <v>0.000919</v>
       </c>
       <c r="F106">
-        <v>0.901457</v>
+        <v>0.750538</v>
       </c>
     </row>
     <row r="107" spans="1:6">
@@ -2205,13 +2205,13 @@
         <v>6</v>
       </c>
       <c r="C107">
-        <v>0.000438</v>
+        <v>0.001701</v>
       </c>
       <c r="D107">
-        <v>3.5E-05</v>
+        <v>0.000271</v>
       </c>
       <c r="F107">
-        <v>0.9189929999999999</v>
+        <v>0.840889</v>
       </c>
     </row>
     <row r="108" spans="1:6">
@@ -2222,13 +2222,13 @@
         <v>6</v>
       </c>
       <c r="C108">
-        <v>0.004297</v>
+        <v>0.021513</v>
       </c>
       <c r="D108">
-        <v>0.001582</v>
+        <v>0.021317</v>
       </c>
       <c r="F108">
-        <v>0.631835</v>
+        <v>0.009082</v>
       </c>
     </row>
     <row r="109" spans="1:6">
@@ -2239,13 +2239,13 @@
         <v>6</v>
       </c>
       <c r="C109">
-        <v>0.002235</v>
+        <v>0.014767</v>
       </c>
       <c r="D109">
-        <v>0.000418</v>
+        <v>0.004971</v>
       </c>
       <c r="F109">
-        <v>0.81298</v>
+        <v>0.663353</v>
       </c>
     </row>
     <row r="110" spans="1:6">
@@ -2256,13 +2256,13 @@
         <v>6</v>
       </c>
       <c r="C110">
-        <v>0.001725</v>
+        <v>0.007919000000000001</v>
       </c>
       <c r="D110">
-        <v>0.000178</v>
+        <v>0.001598</v>
       </c>
       <c r="F110">
-        <v>0.897008</v>
+        <v>0.798143</v>
       </c>
     </row>
     <row r="111" spans="1:6">
@@ -2273,13 +2273,13 @@
         <v>6</v>
       </c>
       <c r="C111">
-        <v>0.000809</v>
+        <v>0.004855</v>
       </c>
       <c r="D111">
-        <v>4.9E-05</v>
+        <v>0.000397</v>
       </c>
       <c r="F111">
-        <v>0.939192</v>
+        <v>0.918156</v>
       </c>
     </row>
     <row r="112" spans="1:6">
@@ -2290,13 +2290,13 @@
         <v>6</v>
       </c>
       <c r="C112">
-        <v>0.000422</v>
+        <v>0.002113</v>
       </c>
       <c r="D112">
-        <v>2.1E-05</v>
+        <v>0.000162</v>
       </c>
       <c r="F112">
-        <v>0.949211</v>
+        <v>0.923271</v>
       </c>
     </row>
     <row r="113" spans="1:6">
@@ -2307,13 +2307,13 @@
         <v>6</v>
       </c>
       <c r="C113">
-        <v>0.002265</v>
+        <v>0.018283</v>
       </c>
       <c r="D113">
-        <v>0.000688</v>
+        <v>0.007993999999999999</v>
       </c>
       <c r="F113">
-        <v>0.696016</v>
+        <v>0.562731</v>
       </c>
     </row>
     <row r="114" spans="1:6">
@@ -2324,13 +2324,13 @@
         <v>6</v>
       </c>
       <c r="C114">
-        <v>0.001305</v>
+        <v>0.010536</v>
       </c>
       <c r="D114">
-        <v>0.000206</v>
+        <v>0.002191</v>
       </c>
       <c r="F114">
-        <v>0.842206</v>
+        <v>0.792048</v>
       </c>
     </row>
     <row r="115" spans="1:6">
@@ -2341,13 +2341,13 @@
         <v>6</v>
       </c>
       <c r="C115">
-        <v>0.000706</v>
+        <v>0.005702</v>
       </c>
       <c r="D115">
-        <v>6.999999999999999E-05</v>
+        <v>0.000645</v>
       </c>
       <c r="F115">
-        <v>0.901178</v>
+        <v>0.88685</v>
       </c>
     </row>
     <row r="116" spans="1:6">
@@ -2358,13 +2358,13 @@
         <v>6</v>
       </c>
       <c r="C116">
-        <v>0.000346</v>
+        <v>0.002797</v>
       </c>
       <c r="D116">
-        <v>2.8E-05</v>
+        <v>0.000236</v>
       </c>
       <c r="F116">
-        <v>0.9199580000000001</v>
+        <v>0.915449</v>
       </c>
     </row>
     <row r="117" spans="1:6">
@@ -2375,13 +2375,13 @@
         <v>6</v>
       </c>
       <c r="C117">
-        <v>0.000152</v>
+        <v>0.001518</v>
       </c>
       <c r="D117">
-        <v>2E-05</v>
+        <v>0.000181</v>
       </c>
       <c r="F117">
-        <v>0.86934</v>
+        <v>0.880722</v>
       </c>
     </row>
     <row r="118" spans="1:6">
@@ -2392,13 +2392,13 @@
         <v>6</v>
       </c>
       <c r="C118">
-        <v>0.001344</v>
+        <v>0.013431</v>
       </c>
       <c r="D118">
-        <v>0.000216</v>
+        <v>0.002566</v>
       </c>
       <c r="F118">
-        <v>0.839272</v>
+        <v>0.808972</v>
       </c>
     </row>
     <row r="119" spans="1:6">
@@ -2409,13 +2409,13 @@
         <v>6</v>
       </c>
       <c r="C119">
-        <v>0.001027</v>
+        <v>0.009209999999999999</v>
       </c>
       <c r="D119">
-        <v>8.899999999999999E-05</v>
+        <v>0.000874</v>
       </c>
       <c r="F119">
-        <v>0.913595</v>
+        <v>0.905085</v>
       </c>
     </row>
     <row r="120" spans="1:6">
@@ -2426,13 +2426,13 @@
         <v>6</v>
       </c>
       <c r="C120">
-        <v>0.000681</v>
+        <v>0.006107</v>
       </c>
       <c r="D120">
-        <v>3.8E-05</v>
+        <v>0.000349</v>
       </c>
       <c r="F120">
-        <v>0.943608</v>
+        <v>0.942865</v>
       </c>
     </row>
     <row r="121" spans="1:6">
@@ -2443,13 +2443,13 @@
         <v>6</v>
       </c>
       <c r="C121">
-        <v>0.000314</v>
+        <v>0.002813</v>
       </c>
       <c r="D121">
-        <v>2.3E-05</v>
+        <v>0.000202</v>
       </c>
       <c r="F121">
-        <v>0.928197</v>
+        <v>0.928055</v>
       </c>
     </row>
     <row r="122" spans="1:6">
@@ -2460,13 +2460,13 @@
         <v>6</v>
       </c>
       <c r="C122">
-        <v>0.001757</v>
+        <v>0.017548</v>
       </c>
       <c r="D122">
-        <v>0.000311</v>
+        <v>0.003573</v>
       </c>
       <c r="F122">
-        <v>0.822765</v>
+        <v>0.796404</v>
       </c>
     </row>
     <row r="123" spans="1:6">
@@ -2477,13 +2477,13 @@
         <v>6</v>
       </c>
       <c r="C123">
-        <v>0.001088</v>
+        <v>0.012173</v>
       </c>
       <c r="D123">
-        <v>0.000119</v>
+        <v>0.001321</v>
       </c>
       <c r="F123">
-        <v>0.890842</v>
+        <v>0.891475</v>
       </c>
     </row>
     <row r="124" spans="1:6">
@@ -2494,13 +2494,13 @@
         <v>6</v>
       </c>
       <c r="C124">
-        <v>0.000694</v>
+        <v>0.007765</v>
       </c>
       <c r="D124">
-        <v>5.3E-05</v>
+        <v>0.000543</v>
       </c>
       <c r="F124">
-        <v>0.923227</v>
+        <v>0.930132</v>
       </c>
     </row>
     <row r="125" spans="1:6">
@@ -2511,13 +2511,13 @@
         <v>6</v>
       </c>
       <c r="C125">
-        <v>0.000326</v>
+        <v>0.003653</v>
       </c>
       <c r="D125">
-        <v>2.9E-05</v>
+        <v>0.000279</v>
       </c>
       <c r="F125">
-        <v>0.912629</v>
+        <v>0.923588</v>
       </c>
     </row>
     <row r="126" spans="1:6">
@@ -2528,13 +2528,13 @@
         <v>6</v>
       </c>
       <c r="C126">
-        <v>0.001303</v>
+        <v>0.021063</v>
       </c>
       <c r="D126">
-        <v>0.000351</v>
+        <v>0.005314</v>
       </c>
       <c r="F126">
-        <v>0.730966</v>
+        <v>0.747718</v>
       </c>
     </row>
     <row r="127" spans="1:6">
@@ -2545,13 +2545,13 @@
         <v>6</v>
       </c>
       <c r="C127">
-        <v>0.000907</v>
+        <v>0.014658</v>
       </c>
       <c r="D127">
-        <v>0.000166</v>
+        <v>0.00229</v>
       </c>
       <c r="F127">
-        <v>0.816629</v>
+        <v>0.843753</v>
       </c>
     </row>
     <row r="128" spans="1:6">
@@ -2562,13 +2562,13 @@
         <v>6</v>
       </c>
       <c r="C128">
-        <v>0.000592</v>
+        <v>0.009572000000000001</v>
       </c>
       <c r="D128">
-        <v>8.3E-05</v>
+        <v>0.001041</v>
       </c>
       <c r="F128">
-        <v>0.8594810000000001</v>
+        <v>0.891271</v>
       </c>
     </row>
     <row r="129" spans="1:6">
@@ -2579,13 +2579,13 @@
         <v>6</v>
       </c>
       <c r="C129">
-        <v>0.000305</v>
+        <v>0.004939</v>
       </c>
       <c r="D129">
-        <v>4.3E-05</v>
+        <v>0.0005</v>
       </c>
       <c r="F129">
-        <v>0.858718</v>
+        <v>0.898711</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Version done for all 4 parts (ready to run)
</commit_message>
<xml_diff>
--- a/part2/tables-2/dom_validty_VER_part-2.xlsx
+++ b/part2/tables-2/dom_validty_VER_part-2.xlsx
@@ -426,13 +426,13 @@
         <v>6</v>
       </c>
       <c r="C2">
-        <v>0.023898</v>
+        <v>0.001723</v>
       </c>
       <c r="D2">
-        <v>0.08387600000000001</v>
+        <v>69.664841</v>
       </c>
       <c r="F2">
-        <v>-2.509709</v>
+        <v>-40438.731661</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -443,13 +443,13 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>0.012234</v>
+        <v>0.00079</v>
       </c>
       <c r="D3">
-        <v>0.017302</v>
+        <v>0.076304</v>
       </c>
       <c r="F3">
-        <v>-0.414278</v>
+        <v>-95.640297</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -460,13 +460,13 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>0.006321</v>
+        <v>0.000359</v>
       </c>
       <c r="D4">
-        <v>0.003263</v>
+        <v>0.001175</v>
       </c>
       <c r="F4">
-        <v>0.48381</v>
+        <v>-2.273466</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -477,13 +477,13 @@
         <v>6</v>
       </c>
       <c r="C5">
-        <v>0.003462</v>
+        <v>0.000188</v>
       </c>
       <c r="D5">
-        <v>0.000669</v>
+        <v>0.000107</v>
       </c>
       <c r="F5">
-        <v>0.80676</v>
+        <v>0.428584</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -494,13 +494,13 @@
         <v>6</v>
       </c>
       <c r="C6">
-        <v>0.029379</v>
+        <v>0.002414</v>
       </c>
       <c r="D6">
-        <v>0.065481</v>
+        <v>106.41218</v>
       </c>
       <c r="F6">
-        <v>-1.228827</v>
+        <v>-44072.360442</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -511,13 +511,13 @@
         <v>6</v>
       </c>
       <c r="C7">
-        <v>0.019388</v>
+        <v>0.001512</v>
       </c>
       <c r="D7">
-        <v>0.015438</v>
+        <v>0.69272</v>
       </c>
       <c r="F7">
-        <v>0.20374</v>
+        <v>-457.057632</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -528,13 +528,13 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <v>0.011025</v>
+        <v>0.000821</v>
       </c>
       <c r="D8">
-        <v>0.004843</v>
+        <v>0.003246</v>
       </c>
       <c r="F8">
-        <v>0.560685</v>
+        <v>-2.955771</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -545,13 +545,13 @@
         <v>6</v>
       </c>
       <c r="C9">
-        <v>0.006425</v>
+        <v>0.000418</v>
       </c>
       <c r="D9">
-        <v>0.000964</v>
+        <v>0.000353</v>
       </c>
       <c r="F9">
-        <v>0.849979</v>
+        <v>0.155365</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -562,13 +562,13 @@
         <v>6</v>
       </c>
       <c r="C10">
-        <v>0.003015</v>
+        <v>0.000177</v>
       </c>
       <c r="D10">
-        <v>0.000287</v>
+        <v>0.002691</v>
       </c>
       <c r="F10">
-        <v>0.904778</v>
+        <v>-14.204</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -579,13 +579,13 @@
         <v>6</v>
       </c>
       <c r="C11">
-        <v>0.022581</v>
+        <v>0.002369</v>
       </c>
       <c r="D11">
-        <v>0.018846</v>
+        <v>1.938189</v>
       </c>
       <c r="F11">
-        <v>0.16541</v>
+        <v>-817.277619</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -596,13 +596,13 @@
         <v>6</v>
       </c>
       <c r="C12">
-        <v>0.013655</v>
+        <v>0.001196</v>
       </c>
       <c r="D12">
-        <v>0.005604</v>
+        <v>0.052778</v>
       </c>
       <c r="F12">
-        <v>0.589615</v>
+        <v>-43.144994</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -613,13 +613,13 @@
         <v>6</v>
       </c>
       <c r="C13">
-        <v>0.00761</v>
+        <v>0.000583</v>
       </c>
       <c r="D13">
-        <v>0.001499</v>
+        <v>0.005828</v>
       </c>
       <c r="F13">
-        <v>0.803023</v>
+        <v>-8.993558</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -630,13 +630,13 @@
         <v>6</v>
       </c>
       <c r="C14">
-        <v>0.003316</v>
+        <v>0.000219</v>
       </c>
       <c r="D14">
-        <v>0.000423</v>
+        <v>0.000928</v>
       </c>
       <c r="F14">
-        <v>0.872564</v>
+        <v>-3.241262</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -647,13 +647,13 @@
         <v>6</v>
       </c>
       <c r="C15">
-        <v>0.002149</v>
+        <v>0.000138</v>
       </c>
       <c r="D15">
-        <v>0.000248</v>
+        <v>0.008177</v>
       </c>
       <c r="F15">
-        <v>0.884486</v>
+        <v>-58.472411</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -664,13 +664,13 @@
         <v>6</v>
       </c>
       <c r="C16">
-        <v>0.015863</v>
+        <v>0.001442</v>
       </c>
       <c r="D16">
-        <v>0.006283</v>
+        <v>0.5106270000000001</v>
       </c>
       <c r="F16">
-        <v>0.603896</v>
+        <v>-353.183669</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -681,13 +681,13 @@
         <v>6</v>
       </c>
       <c r="C17">
-        <v>0.011696</v>
+        <v>0.0009859999999999999</v>
       </c>
       <c r="D17">
-        <v>0.001975</v>
+        <v>0.01559</v>
       </c>
       <c r="F17">
-        <v>0.831171</v>
+        <v>-14.804674</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -698,13 +698,13 @@
         <v>6</v>
       </c>
       <c r="C18">
-        <v>0.006986</v>
+        <v>0.0005330000000000001</v>
       </c>
       <c r="D18">
-        <v>0.0006489999999999999</v>
+        <v>0.004169</v>
       </c>
       <c r="F18">
-        <v>0.907134</v>
+        <v>-6.81789</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -715,13 +715,13 @@
         <v>6</v>
       </c>
       <c r="C19">
-        <v>0.003566</v>
+        <v>0.000253</v>
       </c>
       <c r="D19">
-        <v>0.000295</v>
+        <v>0.002421</v>
       </c>
       <c r="F19">
-        <v>0.917281</v>
+        <v>-8.559036000000001</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -732,13 +732,13 @@
         <v>6</v>
       </c>
       <c r="C20">
-        <v>0.022074</v>
+        <v>0.002366</v>
       </c>
       <c r="D20">
-        <v>0.007860000000000001</v>
+        <v>0.421406</v>
       </c>
       <c r="F20">
-        <v>0.643935</v>
+        <v>-177.124606</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -749,13 +749,13 @@
         <v>6</v>
       </c>
       <c r="C21">
-        <v>0.012619</v>
+        <v>0.001208</v>
       </c>
       <c r="D21">
-        <v>0.002809</v>
+        <v>0.018688</v>
       </c>
       <c r="F21">
-        <v>0.77737</v>
+        <v>-14.47119</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -766,13 +766,13 @@
         <v>6</v>
       </c>
       <c r="C22">
-        <v>0.008056000000000001</v>
+        <v>0.0007</v>
       </c>
       <c r="D22">
-        <v>0.001013</v>
+        <v>0.002208</v>
       </c>
       <c r="F22">
-        <v>0.874245</v>
+        <v>-2.154622</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -783,13 +783,13 @@
         <v>6</v>
       </c>
       <c r="C23">
-        <v>0.004231</v>
+        <v>0.000332</v>
       </c>
       <c r="D23">
-        <v>0.000423</v>
+        <v>0.001038</v>
       </c>
       <c r="F23">
-        <v>0.900037</v>
+        <v>-2.131854</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -800,13 +800,13 @@
         <v>6</v>
       </c>
       <c r="C24">
-        <v>0.023636</v>
+        <v>0.002846</v>
       </c>
       <c r="D24">
-        <v>0.010492</v>
+        <v>0.245524</v>
       </c>
       <c r="F24">
-        <v>0.5560850000000001</v>
+        <v>-85.27987</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -817,13 +817,13 @@
         <v>6</v>
       </c>
       <c r="C25">
-        <v>0.016717</v>
+        <v>0.001858</v>
       </c>
       <c r="D25">
-        <v>0.004479</v>
+        <v>0.008475999999999999</v>
       </c>
       <c r="F25">
-        <v>0.732043</v>
+        <v>-3.561121</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -834,13 +834,13 @@
         <v>6</v>
       </c>
       <c r="C26">
-        <v>0.009950000000000001</v>
+        <v>0.001024</v>
       </c>
       <c r="D26">
-        <v>0.001894</v>
+        <v>0.000754</v>
       </c>
       <c r="F26">
-        <v>0.809602</v>
+        <v>0.26426</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -851,13 +851,13 @@
         <v>6</v>
       </c>
       <c r="C27">
-        <v>0.005314</v>
+        <v>0.000489</v>
       </c>
       <c r="D27">
-        <v>0.000791</v>
+        <v>0.002012</v>
       </c>
       <c r="F27">
-        <v>0.851108</v>
+        <v>-3.111564</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -868,13 +868,13 @@
         <v>6</v>
       </c>
       <c r="C28">
-        <v>0.024311</v>
+        <v>0.001752</v>
       </c>
       <c r="D28">
-        <v>0.08387600000000001</v>
+        <v>69.664841</v>
       </c>
       <c r="F28">
-        <v>-2.450156</v>
+        <v>-39752.542259</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -885,13 +885,13 @@
         <v>6</v>
       </c>
       <c r="C29">
-        <v>0.013068</v>
+        <v>0.000843</v>
       </c>
       <c r="D29">
-        <v>0.017302</v>
+        <v>0.076304</v>
       </c>
       <c r="F29">
-        <v>-0.324005</v>
+        <v>-89.471768</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -902,13 +902,13 @@
         <v>6</v>
       </c>
       <c r="C30">
-        <v>0.006005</v>
+        <v>0.000341</v>
       </c>
       <c r="D30">
-        <v>0.003263</v>
+        <v>0.001175</v>
       </c>
       <c r="F30">
-        <v>0.456643</v>
+        <v>-2.445754</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -919,13 +919,13 @@
         <v>6</v>
       </c>
       <c r="C31">
-        <v>0.003434</v>
+        <v>0.000186</v>
       </c>
       <c r="D31">
-        <v>0.000669</v>
+        <v>0.000107</v>
       </c>
       <c r="F31">
-        <v>0.805163</v>
+        <v>0.423861</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -936,13 +936,13 @@
         <v>6</v>
       </c>
       <c r="C32">
-        <v>0.02868</v>
+        <v>0.002357</v>
       </c>
       <c r="D32">
-        <v>0.065481</v>
+        <v>106.41218</v>
       </c>
       <c r="F32">
-        <v>-1.283191</v>
+        <v>-45147.380844</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -953,13 +953,13 @@
         <v>6</v>
       </c>
       <c r="C33">
-        <v>0.019317</v>
+        <v>0.001507</v>
       </c>
       <c r="D33">
-        <v>0.015438</v>
+        <v>0.69272</v>
       </c>
       <c r="F33">
-        <v>0.200824</v>
+        <v>-458.73486</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -970,13 +970,13 @@
         <v>6</v>
       </c>
       <c r="C34">
-        <v>0.010519</v>
+        <v>0.000783</v>
       </c>
       <c r="D34">
-        <v>0.004843</v>
+        <v>0.003246</v>
       </c>
       <c r="F34">
-        <v>0.539531</v>
+        <v>-3.146249</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -987,13 +987,13 @@
         <v>6</v>
       </c>
       <c r="C35">
-        <v>0.005846</v>
+        <v>0.000381</v>
       </c>
       <c r="D35">
-        <v>0.000964</v>
+        <v>0.000353</v>
       </c>
       <c r="F35">
-        <v>0.835121</v>
+        <v>0.071715</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1004,13 +1004,13 @@
         <v>6</v>
       </c>
       <c r="C36">
-        <v>0.003195</v>
+        <v>0.000188</v>
       </c>
       <c r="D36">
-        <v>0.000287</v>
+        <v>0.002691</v>
       </c>
       <c r="F36">
-        <v>0.910145</v>
+        <v>-13.347008</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1021,13 +1021,13 @@
         <v>6</v>
       </c>
       <c r="C37">
-        <v>0.022656</v>
+        <v>0.002376</v>
       </c>
       <c r="D37">
-        <v>0.018846</v>
+        <v>1.938189</v>
       </c>
       <c r="F37">
-        <v>0.168171</v>
+        <v>-814.571238</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1038,13 +1038,13 @@
         <v>6</v>
       </c>
       <c r="C38">
-        <v>0.013821</v>
+        <v>0.00121</v>
       </c>
       <c r="D38">
-        <v>0.005604</v>
+        <v>0.052778</v>
       </c>
       <c r="F38">
-        <v>0.5945589999999999</v>
+        <v>-42.613126</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1055,13 +1055,13 @@
         <v>6</v>
       </c>
       <c r="C39">
-        <v>0.00761</v>
+        <v>0.000583</v>
       </c>
       <c r="D39">
-        <v>0.001499</v>
+        <v>0.005828</v>
       </c>
       <c r="F39">
-        <v>0.803023</v>
+        <v>-8.993558</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1072,13 +1072,13 @@
         <v>6</v>
       </c>
       <c r="C40">
-        <v>0.003316</v>
+        <v>0.000219</v>
       </c>
       <c r="D40">
-        <v>0.000423</v>
+        <v>0.000928</v>
       </c>
       <c r="F40">
-        <v>0.872564</v>
+        <v>-3.241262</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1089,13 +1089,13 @@
         <v>6</v>
       </c>
       <c r="C41">
-        <v>0.002188</v>
+        <v>0.00014</v>
       </c>
       <c r="D41">
-        <v>0.000248</v>
+        <v>0.008177</v>
       </c>
       <c r="F41">
-        <v>0.886549</v>
+        <v>-57.410404</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1106,13 +1106,13 @@
         <v>6</v>
       </c>
       <c r="C42">
-        <v>0.015863</v>
+        <v>0.001442</v>
       </c>
       <c r="D42">
-        <v>0.006283</v>
+        <v>0.5106270000000001</v>
       </c>
       <c r="F42">
-        <v>0.603896</v>
+        <v>-353.183669</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1123,13 +1123,13 @@
         <v>6</v>
       </c>
       <c r="C43">
-        <v>0.011538</v>
+        <v>0.000973</v>
       </c>
       <c r="D43">
-        <v>0.001975</v>
+        <v>0.01559</v>
       </c>
       <c r="F43">
-        <v>0.828858</v>
+        <v>-15.021177</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1140,13 +1140,13 @@
         <v>6</v>
       </c>
       <c r="C44">
-        <v>0.006986</v>
+        <v>0.0005330000000000001</v>
       </c>
       <c r="D44">
-        <v>0.0006489999999999999</v>
+        <v>0.004169</v>
       </c>
       <c r="F44">
-        <v>0.907134</v>
+        <v>-6.81789</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1157,13 +1157,13 @@
         <v>6</v>
       </c>
       <c r="C45">
-        <v>0.003379</v>
+        <v>0.00024</v>
       </c>
       <c r="D45">
-        <v>0.000295</v>
+        <v>0.002421</v>
       </c>
       <c r="F45">
-        <v>0.912686</v>
+        <v>-9.090093</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1174,13 +1174,13 @@
         <v>6</v>
       </c>
       <c r="C46">
-        <v>0.021766</v>
+        <v>0.002333</v>
       </c>
       <c r="D46">
-        <v>0.007860000000000001</v>
+        <v>0.421406</v>
       </c>
       <c r="F46">
-        <v>0.638891</v>
+        <v>-179.647804</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1191,13 +1191,13 @@
         <v>6</v>
       </c>
       <c r="C47">
-        <v>0.013369</v>
+        <v>0.00128</v>
       </c>
       <c r="D47">
-        <v>0.002809</v>
+        <v>0.018688</v>
       </c>
       <c r="F47">
-        <v>0.78986</v>
+        <v>-13.603196</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1208,13 +1208,13 @@
         <v>6</v>
       </c>
       <c r="C48">
-        <v>0.007773</v>
+        <v>0.000675</v>
       </c>
       <c r="D48">
-        <v>0.001013</v>
+        <v>0.002208</v>
       </c>
       <c r="F48">
-        <v>0.869672</v>
+        <v>-2.269336</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1225,13 +1225,13 @@
         <v>6</v>
       </c>
       <c r="C49">
-        <v>0.003918</v>
+        <v>0.000307</v>
       </c>
       <c r="D49">
-        <v>0.000423</v>
+        <v>0.001038</v>
       </c>
       <c r="F49">
-        <v>0.8920400000000001</v>
+        <v>-2.382402</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1242,13 +1242,13 @@
         <v>6</v>
       </c>
       <c r="C50">
-        <v>0.023686</v>
+        <v>0.002852</v>
       </c>
       <c r="D50">
-        <v>0.010492</v>
+        <v>0.245524</v>
       </c>
       <c r="F50">
-        <v>0.55704</v>
+        <v>-85.09427100000001</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1259,13 +1259,13 @@
         <v>6</v>
       </c>
       <c r="C51">
-        <v>0.016512</v>
+        <v>0.001836</v>
       </c>
       <c r="D51">
-        <v>0.004479</v>
+        <v>0.008475999999999999</v>
       </c>
       <c r="F51">
-        <v>0.728721</v>
+        <v>-3.617674</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -1276,13 +1276,13 @@
         <v>6</v>
       </c>
       <c r="C52">
-        <v>0.009508000000000001</v>
+        <v>0.0009790000000000001</v>
       </c>
       <c r="D52">
-        <v>0.001894</v>
+        <v>0.000754</v>
       </c>
       <c r="F52">
-        <v>0.800746</v>
+        <v>0.23004</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -1293,13 +1293,13 @@
         <v>6</v>
       </c>
       <c r="C53">
-        <v>0.005067</v>
+        <v>0.000467</v>
       </c>
       <c r="D53">
-        <v>0.000791</v>
+        <v>0.002012</v>
       </c>
       <c r="F53">
-        <v>0.843845</v>
+        <v>-3.312128</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -1310,13 +1310,13 @@
         <v>6</v>
       </c>
       <c r="C54">
-        <v>0.026871</v>
+        <v>0.001937</v>
       </c>
       <c r="D54">
-        <v>0.110449</v>
+        <v>250.341638</v>
       </c>
       <c r="F54">
-        <v>-3.110411</v>
+        <v>-129245.415778</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -1327,13 +1327,13 @@
         <v>6</v>
       </c>
       <c r="C55">
-        <v>0.01242</v>
+        <v>0.000802</v>
       </c>
       <c r="D55">
-        <v>0.02357</v>
+        <v>0.206562</v>
       </c>
       <c r="F55">
-        <v>-0.897742</v>
+        <v>-256.694774</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -1344,13 +1344,13 @@
         <v>6</v>
       </c>
       <c r="C56">
-        <v>0.006224</v>
+        <v>0.000353</v>
       </c>
       <c r="D56">
-        <v>0.004465</v>
+        <v>0.002185</v>
       </c>
       <c r="F56">
-        <v>0.282678</v>
+        <v>-5.183798</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -1361,13 +1361,13 @@
         <v>6</v>
       </c>
       <c r="C57">
-        <v>0.00293</v>
+        <v>0.000159</v>
       </c>
       <c r="D57">
-        <v>0.000857</v>
+        <v>0.000109</v>
       </c>
       <c r="F57">
-        <v>0.7075090000000001</v>
+        <v>0.315803</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -1378,13 +1378,13 @@
         <v>6</v>
       </c>
       <c r="C58">
-        <v>0.033065</v>
+        <v>0.002717</v>
       </c>
       <c r="D58">
-        <v>0.083442</v>
+        <v>436.561879</v>
       </c>
       <c r="F58">
-        <v>-1.523598</v>
+        <v>-160658.179512</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -1395,13 +1395,13 @@
         <v>6</v>
       </c>
       <c r="C59">
-        <v>0.021233</v>
+        <v>0.001656</v>
       </c>
       <c r="D59">
-        <v>0.019911</v>
+        <v>1.85983</v>
       </c>
       <c r="F59">
-        <v>0.062236</v>
+        <v>-1121.950623</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -1412,13 +1412,13 @@
         <v>6</v>
       </c>
       <c r="C60">
-        <v>0.011816</v>
+        <v>0.000879</v>
       </c>
       <c r="D60">
-        <v>0.006295</v>
+        <v>0.005169</v>
       </c>
       <c r="F60">
-        <v>0.46724</v>
+        <v>-4.877826</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -1429,13 +1429,13 @@
         <v>6</v>
       </c>
       <c r="C61">
-        <v>0.006512</v>
+        <v>0.000424</v>
       </c>
       <c r="D61">
-        <v>0.001214</v>
+        <v>0.00058</v>
       </c>
       <c r="F61">
-        <v>0.813593</v>
+        <v>-0.367476</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -1446,13 +1446,13 @@
         <v>6</v>
       </c>
       <c r="C62">
-        <v>0.002817</v>
+        <v>0.000165</v>
       </c>
       <c r="D62">
-        <v>0.000338</v>
+        <v>0.001258</v>
       </c>
       <c r="F62">
-        <v>0.8799129999999999</v>
+        <v>-6.607175</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -1463,13 +1463,13 @@
         <v>6</v>
       </c>
       <c r="C63">
-        <v>0.024135</v>
+        <v>0.002532</v>
       </c>
       <c r="D63">
-        <v>0.022779</v>
+        <v>4.487569</v>
       </c>
       <c r="F63">
-        <v>0.056193</v>
+        <v>-1771.552265</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -1480,13 +1480,13 @@
         <v>6</v>
       </c>
       <c r="C64">
-        <v>0.015479</v>
+        <v>0.001355</v>
       </c>
       <c r="D64">
-        <v>0.006966</v>
+        <v>0.146471</v>
       </c>
       <c r="F64">
-        <v>0.549949</v>
+        <v>-107.074461</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -1497,13 +1497,13 @@
         <v>6</v>
       </c>
       <c r="C65">
-        <v>0.007865</v>
+        <v>0.000603</v>
       </c>
       <c r="D65">
-        <v>0.00185</v>
+        <v>0.006699</v>
       </c>
       <c r="F65">
-        <v>0.764798</v>
+        <v>-10.1144</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -1514,13 +1514,13 @@
         <v>6</v>
       </c>
       <c r="C66">
-        <v>0.003617</v>
+        <v>0.000239</v>
       </c>
       <c r="D66">
-        <v>0.000497</v>
+        <v>0.001188</v>
       </c>
       <c r="F66">
-        <v>0.862667</v>
+        <v>-3.978057</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -1531,13 +1531,13 @@
         <v>6</v>
       </c>
       <c r="C67">
-        <v>0.00244</v>
+        <v>0.000156</v>
       </c>
       <c r="D67">
-        <v>0.000274</v>
+        <v>0.002811</v>
       </c>
       <c r="F67">
-        <v>0.887834</v>
+        <v>-17.010621</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -1548,13 +1548,13 @@
         <v>6</v>
       </c>
       <c r="C68">
-        <v>0.018273</v>
+        <v>0.001661</v>
       </c>
       <c r="D68">
-        <v>0.007723</v>
+        <v>1.125433</v>
       </c>
       <c r="F68">
-        <v>0.577353</v>
+        <v>-676.639654</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -1565,13 +1565,13 @@
         <v>6</v>
       </c>
       <c r="C69">
-        <v>0.012323</v>
+        <v>0.001039</v>
       </c>
       <c r="D69">
-        <v>0.002409</v>
+        <v>0.018783</v>
       </c>
       <c r="F69">
-        <v>0.804536</v>
+        <v>-17.071453</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -1582,13 +1582,13 @@
         <v>6</v>
       </c>
       <c r="C70">
-        <v>0.007802</v>
+        <v>0.000595</v>
       </c>
       <c r="D70">
-        <v>0.0007649999999999999</v>
+        <v>0.00503</v>
       </c>
       <c r="F70">
-        <v>0.901999</v>
+        <v>-7.447163</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -1599,13 +1599,13 @@
         <v>6</v>
       </c>
       <c r="C71">
-        <v>0.004322</v>
+        <v>0.000307</v>
       </c>
       <c r="D71">
-        <v>0.000329</v>
+        <v>0.001812</v>
       </c>
       <c r="F71">
-        <v>0.923833</v>
+        <v>-4.905066</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -1616,13 +1616,13 @@
         <v>6</v>
       </c>
       <c r="C72">
-        <v>0.023986</v>
+        <v>0.002571</v>
       </c>
       <c r="D72">
-        <v>0.009398999999999999</v>
+        <v>0.88392</v>
       </c>
       <c r="F72">
-        <v>0.608127</v>
+        <v>-342.847414</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -1633,13 +1633,13 @@
         <v>6</v>
       </c>
       <c r="C73">
-        <v>0.01534</v>
+        <v>0.001468</v>
       </c>
       <c r="D73">
-        <v>0.003362</v>
+        <v>0.030437</v>
       </c>
       <c r="F73">
-        <v>0.780818</v>
+        <v>-19.72818</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -1650,13 +1650,13 @@
         <v>6</v>
       </c>
       <c r="C74">
-        <v>0.009372</v>
+        <v>0.0008140000000000001</v>
       </c>
       <c r="D74">
-        <v>0.001188</v>
+        <v>0.002695</v>
       </c>
       <c r="F74">
-        <v>0.873289</v>
+        <v>-2.310545</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -1667,13 +1667,13 @@
         <v>6</v>
       </c>
       <c r="C75">
-        <v>0.004913</v>
+        <v>0.000385</v>
       </c>
       <c r="D75">
-        <v>0.000475</v>
+        <v>0.00088</v>
       </c>
       <c r="F75">
-        <v>0.903323</v>
+        <v>-1.28541</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -1684,13 +1684,13 @@
         <v>6</v>
       </c>
       <c r="C76">
-        <v>0.026495</v>
+        <v>0.00319</v>
       </c>
       <c r="D76">
-        <v>0.012224</v>
+        <v>0.390739</v>
       </c>
       <c r="F76">
-        <v>0.538642</v>
+        <v>-121.490069</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -1701,13 +1701,13 @@
         <v>6</v>
       </c>
       <c r="C77">
-        <v>0.018404</v>
+        <v>0.002046</v>
       </c>
       <c r="D77">
-        <v>0.005235</v>
+        <v>0.016942</v>
       </c>
       <c r="F77">
-        <v>0.71557</v>
+        <v>-7.28086</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -1718,13 +1718,13 @@
         <v>6</v>
       </c>
       <c r="C78">
-        <v>0.011565</v>
+        <v>0.00119</v>
       </c>
       <c r="D78">
-        <v>0.002192</v>
+        <v>0.000965</v>
       </c>
       <c r="F78">
-        <v>0.810457</v>
+        <v>0.189221</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -1735,13 +1735,13 @@
         <v>6</v>
       </c>
       <c r="C79">
-        <v>0.00655</v>
+        <v>0.000603</v>
       </c>
       <c r="D79">
-        <v>0.000892</v>
+        <v>0.001633</v>
       </c>
       <c r="F79">
-        <v>0.863754</v>
+        <v>-1.707875</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -1749,13 +1749,13 @@
         <v>79</v>
       </c>
       <c r="C80">
-        <v>0.023147</v>
+        <v>0.001494</v>
       </c>
       <c r="D80">
-        <v>0.093061</v>
+        <v>35.68684</v>
       </c>
       <c r="F80">
-        <v>-3.020344</v>
+        <v>-23887.544839</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -1766,13 +1766,13 @@
         <v>6</v>
       </c>
       <c r="C81">
-        <v>0.012102</v>
+        <v>0.000687</v>
       </c>
       <c r="D81">
-        <v>0.019805</v>
+        <v>0.060415</v>
       </c>
       <c r="F81">
-        <v>-0.636468</v>
+        <v>-86.91664</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -1783,13 +1783,13 @@
         <v>6</v>
       </c>
       <c r="C82">
-        <v>0.006614</v>
+        <v>0.000359</v>
       </c>
       <c r="D82">
-        <v>0.003148</v>
+        <v>0.001361</v>
       </c>
       <c r="F82">
-        <v>0.524004</v>
+        <v>-2.795161</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -1800,13 +1800,13 @@
         <v>6</v>
       </c>
       <c r="C83">
-        <v>0.031251</v>
+        <v>0.002438</v>
       </c>
       <c r="D83">
-        <v>0.061462</v>
+        <v>81.39379099999999</v>
       </c>
       <c r="F83">
-        <v>-0.966744</v>
+        <v>-33389.747364</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -1814,13 +1814,13 @@
         <v>84</v>
       </c>
       <c r="C84">
-        <v>0.017637</v>
+        <v>0.001313</v>
       </c>
       <c r="D84">
-        <v>0.021105</v>
+        <v>0.316211</v>
       </c>
       <c r="F84">
-        <v>-0.196659</v>
+        <v>-239.911305</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -1831,13 +1831,13 @@
         <v>6</v>
       </c>
       <c r="C85">
-        <v>0.010697</v>
+        <v>0.000696</v>
       </c>
       <c r="D85">
-        <v>0.003875</v>
+        <v>0.006842</v>
       </c>
       <c r="F85">
-        <v>0.63775</v>
+        <v>-8.824184000000001</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -1848,13 +1848,13 @@
         <v>6</v>
       </c>
       <c r="C86">
-        <v>0.005932</v>
+        <v>0.000348</v>
       </c>
       <c r="D86">
-        <v>0.000851</v>
+        <v>0.000232</v>
       </c>
       <c r="F86">
-        <v>0.856525</v>
+        <v>0.334044</v>
       </c>
     </row>
     <row r="87" spans="1:6">
@@ -1865,13 +1865,13 @@
         <v>6</v>
       </c>
       <c r="C87">
-        <v>0.03393</v>
+        <v>0.003559</v>
       </c>
       <c r="D87">
-        <v>0.0525</v>
+        <v>242.47813</v>
       </c>
       <c r="F87">
-        <v>-0.547289</v>
+        <v>-68127.343958</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -1882,13 +1882,13 @@
         <v>6</v>
       </c>
       <c r="C88">
-        <v>0.021071</v>
+        <v>0.001845</v>
       </c>
       <c r="D88">
-        <v>0.018818</v>
+        <v>6.508854</v>
       </c>
       <c r="F88">
-        <v>0.106956</v>
+        <v>-3526.92344</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -1899,13 +1899,13 @@
         <v>6</v>
       </c>
       <c r="C89">
-        <v>0.012037</v>
+        <v>0.000922</v>
       </c>
       <c r="D89">
-        <v>0.005144</v>
+        <v>0.144214</v>
       </c>
       <c r="F89">
-        <v>0.5726830000000001</v>
+        <v>-155.333244</v>
       </c>
     </row>
     <row r="90" spans="1:6">
@@ -1916,13 +1916,13 @@
         <v>6</v>
       </c>
       <c r="C90">
-        <v>0.006625</v>
+        <v>0.000437</v>
       </c>
       <c r="D90">
-        <v>0.001193</v>
+        <v>0.003423</v>
       </c>
       <c r="F90">
-        <v>0.819873</v>
+        <v>-6.833103</v>
       </c>
     </row>
     <row r="91" spans="1:6">
@@ -1933,13 +1933,13 @@
         <v>6</v>
       </c>
       <c r="C91">
-        <v>0.004173</v>
+        <v>0.000267</v>
       </c>
       <c r="D91">
-        <v>0.00049</v>
+        <v>0.000613</v>
       </c>
       <c r="F91">
-        <v>0.88269</v>
+        <v>-1.295538</v>
       </c>
     </row>
     <row r="92" spans="1:6">
@@ -1950,13 +1950,13 @@
         <v>6</v>
       </c>
       <c r="C92">
-        <v>0.028196</v>
+        <v>0.002563</v>
       </c>
       <c r="D92">
-        <v>0.019747</v>
+        <v>14.973982</v>
       </c>
       <c r="F92">
-        <v>0.299649</v>
+        <v>-5842.171933</v>
       </c>
     </row>
     <row r="93" spans="1:6">
@@ -1967,13 +1967,13 @@
         <v>6</v>
       </c>
       <c r="C93">
-        <v>0.017105</v>
+        <v>0.001443</v>
       </c>
       <c r="D93">
-        <v>0.006227</v>
+        <v>0.403521</v>
       </c>
       <c r="F93">
-        <v>0.635961</v>
+        <v>-278.703966</v>
       </c>
     </row>
     <row r="94" spans="1:6">
@@ -1984,13 +1984,13 @@
         <v>6</v>
       </c>
       <c r="C94">
-        <v>0.01076</v>
+        <v>0.000821</v>
       </c>
       <c r="D94">
-        <v>0.001785</v>
+        <v>0.011747</v>
       </c>
       <c r="F94">
-        <v>0.834066</v>
+        <v>-13.305065</v>
       </c>
     </row>
     <row r="95" spans="1:6">
@@ -2001,13 +2001,13 @@
         <v>6</v>
       </c>
       <c r="C95">
-        <v>0.005626</v>
+        <v>0.0004</v>
       </c>
       <c r="D95">
-        <v>0.000613</v>
+        <v>0.002541</v>
       </c>
       <c r="F95">
-        <v>0.890999</v>
+        <v>-5.360025</v>
       </c>
     </row>
     <row r="96" spans="1:6">
@@ -2018,13 +2018,13 @@
         <v>6</v>
       </c>
       <c r="C96">
-        <v>0.028537</v>
+        <v>0.003058</v>
       </c>
       <c r="D96">
-        <v>0.021048</v>
+        <v>10.451209</v>
       </c>
       <c r="F96">
-        <v>0.262451</v>
+        <v>-3416.106856</v>
       </c>
     </row>
     <row r="97" spans="1:6">
@@ -2035,13 +2035,13 @@
         <v>6</v>
       </c>
       <c r="C97">
-        <v>0.020075</v>
+        <v>0.001922</v>
       </c>
       <c r="D97">
-        <v>0.007811</v>
+        <v>0.721374</v>
       </c>
       <c r="F97">
-        <v>0.610895</v>
+        <v>-374.400442</v>
       </c>
     </row>
     <row r="98" spans="1:6">
@@ -2052,13 +2052,13 @@
         <v>6</v>
       </c>
       <c r="C98">
-        <v>0.012707</v>
+        <v>0.001104</v>
       </c>
       <c r="D98">
-        <v>0.002624</v>
+        <v>0.011045</v>
       </c>
       <c r="F98">
-        <v>0.793531</v>
+        <v>-9.005767000000001</v>
       </c>
     </row>
     <row r="99" spans="1:6">
@@ -2069,13 +2069,13 @@
         <v>6</v>
       </c>
       <c r="C99">
-        <v>0.006784</v>
+        <v>0.000532</v>
       </c>
       <c r="D99">
-        <v>0.000894</v>
+        <v>0.001012</v>
       </c>
       <c r="F99">
-        <v>0.868291</v>
+        <v>-0.903819</v>
       </c>
     </row>
     <row r="100" spans="1:6">
@@ -2086,13 +2086,13 @@
         <v>6</v>
       </c>
       <c r="C100">
-        <v>0.031981</v>
+        <v>0.003851</v>
       </c>
       <c r="D100">
-        <v>0.024237</v>
+        <v>1.998099</v>
       </c>
       <c r="F100">
-        <v>0.242164</v>
+        <v>-517.918446</v>
       </c>
     </row>
     <row r="101" spans="1:6">
@@ -2103,13 +2103,13 @@
         <v>6</v>
       </c>
       <c r="C101">
-        <v>0.023206</v>
+        <v>0.00258</v>
       </c>
       <c r="D101">
-        <v>0.010733</v>
+        <v>0.279611</v>
       </c>
       <c r="F101">
-        <v>0.537498</v>
+        <v>-107.390683</v>
       </c>
     </row>
     <row r="102" spans="1:6">
@@ -2120,13 +2120,13 @@
         <v>6</v>
       </c>
       <c r="C102">
-        <v>0.015462</v>
+        <v>0.001592</v>
       </c>
       <c r="D102">
-        <v>0.00442</v>
+        <v>0.009113</v>
       </c>
       <c r="F102">
-        <v>0.714112</v>
+        <v>-4.726032</v>
       </c>
     </row>
     <row r="103" spans="1:6">
@@ -2137,13 +2137,13 @@
         <v>6</v>
       </c>
       <c r="C103">
-        <v>0.008643</v>
+        <v>0.000796</v>
       </c>
       <c r="D103">
-        <v>0.001657</v>
+        <v>0.001381</v>
       </c>
       <c r="F103">
-        <v>0.808248</v>
+        <v>-0.735033</v>
       </c>
     </row>
     <row r="104" spans="1:6">
@@ -2154,13 +2154,13 @@
         <v>6</v>
       </c>
       <c r="C104">
-        <v>0.016497</v>
+        <v>0.001189</v>
       </c>
       <c r="D104">
-        <v>0.023491</v>
+        <v>0.564934</v>
       </c>
       <c r="F104">
-        <v>-0.424011</v>
+        <v>-474.079488</v>
       </c>
     </row>
     <row r="105" spans="1:6">
@@ -2171,13 +2171,13 @@
         <v>6</v>
       </c>
       <c r="C105">
-        <v>0.007407</v>
+        <v>0.000478</v>
       </c>
       <c r="D105">
-        <v>0.004434</v>
+        <v>0.003134</v>
       </c>
       <c r="F105">
-        <v>0.401381</v>
+        <v>-5.555445</v>
       </c>
     </row>
     <row r="106" spans="1:6">
@@ -2188,13 +2188,13 @@
         <v>6</v>
       </c>
       <c r="C106">
-        <v>0.003683</v>
+        <v>0.000209</v>
       </c>
       <c r="D106">
-        <v>0.000919</v>
+        <v>6.999999999999999E-05</v>
       </c>
       <c r="F106">
-        <v>0.750538</v>
+        <v>0.664498</v>
       </c>
     </row>
     <row r="107" spans="1:6">
@@ -2205,13 +2205,13 @@
         <v>6</v>
       </c>
       <c r="C107">
-        <v>0.001701</v>
+        <v>9.2E-05</v>
       </c>
       <c r="D107">
-        <v>0.000271</v>
+        <v>0.001868</v>
       </c>
       <c r="F107">
-        <v>0.840889</v>
+        <v>-19.256899</v>
       </c>
     </row>
     <row r="108" spans="1:6">
@@ -2222,13 +2222,13 @@
         <v>6</v>
       </c>
       <c r="C108">
-        <v>0.021513</v>
+        <v>0.001768</v>
       </c>
       <c r="D108">
-        <v>0.021317</v>
+        <v>0.369708</v>
       </c>
       <c r="F108">
-        <v>0.009082</v>
+        <v>-208.117613</v>
       </c>
     </row>
     <row r="109" spans="1:6">
@@ -2239,13 +2239,13 @@
         <v>6</v>
       </c>
       <c r="C109">
-        <v>0.014767</v>
+        <v>0.001152</v>
       </c>
       <c r="D109">
-        <v>0.004971</v>
+        <v>0.008866000000000001</v>
       </c>
       <c r="F109">
-        <v>0.663353</v>
+        <v>-6.697134</v>
       </c>
     </row>
     <row r="110" spans="1:6">
@@ -2256,13 +2256,13 @@
         <v>6</v>
       </c>
       <c r="C110">
-        <v>0.007919000000000001</v>
+        <v>0.000589</v>
       </c>
       <c r="D110">
-        <v>0.001598</v>
+        <v>0.001281</v>
       </c>
       <c r="F110">
-        <v>0.798143</v>
+        <v>-1.174256</v>
       </c>
     </row>
     <row r="111" spans="1:6">
@@ -2273,13 +2273,13 @@
         <v>6</v>
       </c>
       <c r="C111">
-        <v>0.004855</v>
+        <v>0.000316</v>
       </c>
       <c r="D111">
-        <v>0.000397</v>
+        <v>0.000427</v>
       </c>
       <c r="F111">
-        <v>0.918156</v>
+        <v>-0.349723</v>
       </c>
     </row>
     <row r="112" spans="1:6">
@@ -2290,13 +2290,13 @@
         <v>6</v>
       </c>
       <c r="C112">
-        <v>0.002113</v>
+        <v>0.000124</v>
       </c>
       <c r="D112">
-        <v>0.000162</v>
+        <v>0.006666</v>
       </c>
       <c r="F112">
-        <v>0.923271</v>
+        <v>-52.750081</v>
       </c>
     </row>
     <row r="113" spans="1:6">
@@ -2307,13 +2307,13 @@
         <v>6</v>
       </c>
       <c r="C113">
-        <v>0.018283</v>
+        <v>0.001918</v>
       </c>
       <c r="D113">
-        <v>0.007993999999999999</v>
+        <v>0.03176</v>
       </c>
       <c r="F113">
-        <v>0.562731</v>
+        <v>-15.561007</v>
       </c>
     </row>
     <row r="114" spans="1:6">
@@ -2324,13 +2324,13 @@
         <v>6</v>
       </c>
       <c r="C114">
-        <v>0.010536</v>
+        <v>0.000922</v>
       </c>
       <c r="D114">
-        <v>0.002191</v>
+        <v>0.004791</v>
       </c>
       <c r="F114">
-        <v>0.792048</v>
+        <v>-4.193879</v>
       </c>
     </row>
     <row r="115" spans="1:6">
@@ -2341,13 +2341,13 @@
         <v>6</v>
       </c>
       <c r="C115">
-        <v>0.005702</v>
+        <v>0.000437</v>
       </c>
       <c r="D115">
-        <v>0.000645</v>
+        <v>0.002666</v>
       </c>
       <c r="F115">
-        <v>0.88685</v>
+        <v>-5.101084</v>
       </c>
     </row>
     <row r="116" spans="1:6">
@@ -2358,13 +2358,13 @@
         <v>6</v>
       </c>
       <c r="C116">
-        <v>0.002797</v>
+        <v>0.000184</v>
       </c>
       <c r="D116">
-        <v>0.000236</v>
+        <v>0.004271</v>
       </c>
       <c r="F116">
-        <v>0.915449</v>
+        <v>-22.147261</v>
       </c>
     </row>
     <row r="117" spans="1:6">
@@ -2375,13 +2375,13 @@
         <v>6</v>
       </c>
       <c r="C117">
-        <v>0.001518</v>
+        <v>9.7E-05</v>
       </c>
       <c r="D117">
-        <v>0.000181</v>
+        <v>0.13357</v>
       </c>
       <c r="F117">
-        <v>0.880722</v>
+        <v>-1374.556355</v>
       </c>
     </row>
     <row r="118" spans="1:6">
@@ -2392,13 +2392,13 @@
         <v>6</v>
       </c>
       <c r="C118">
-        <v>0.013431</v>
+        <v>0.001221</v>
       </c>
       <c r="D118">
-        <v>0.002566</v>
+        <v>0.024779</v>
       </c>
       <c r="F118">
-        <v>0.808972</v>
+        <v>-19.298968</v>
       </c>
     </row>
     <row r="119" spans="1:6">
@@ -2409,13 +2409,13 @@
         <v>6</v>
       </c>
       <c r="C119">
-        <v>0.009209999999999999</v>
+        <v>0.000777</v>
       </c>
       <c r="D119">
-        <v>0.000874</v>
+        <v>0.008263</v>
       </c>
       <c r="F119">
-        <v>0.905085</v>
+        <v>-9.636913</v>
       </c>
     </row>
     <row r="120" spans="1:6">
@@ -2426,13 +2426,13 @@
         <v>6</v>
       </c>
       <c r="C120">
-        <v>0.006107</v>
+        <v>0.000466</v>
       </c>
       <c r="D120">
-        <v>0.000349</v>
+        <v>0.002256</v>
       </c>
       <c r="F120">
-        <v>0.942865</v>
+        <v>-3.840598</v>
       </c>
     </row>
     <row r="121" spans="1:6">
@@ -2443,13 +2443,13 @@
         <v>6</v>
       </c>
       <c r="C121">
-        <v>0.002813</v>
+        <v>0.0002</v>
       </c>
       <c r="D121">
-        <v>0.000202</v>
+        <v>0.029122</v>
       </c>
       <c r="F121">
-        <v>0.928055</v>
+        <v>-144.78775</v>
       </c>
     </row>
     <row r="122" spans="1:6">
@@ -2460,13 +2460,13 @@
         <v>6</v>
       </c>
       <c r="C122">
-        <v>0.017548</v>
+        <v>0.001881</v>
       </c>
       <c r="D122">
-        <v>0.003573</v>
+        <v>0.028715</v>
       </c>
       <c r="F122">
-        <v>0.796404</v>
+        <v>-14.267781</v>
       </c>
     </row>
     <row r="123" spans="1:6">
@@ -2477,13 +2477,13 @@
         <v>6</v>
       </c>
       <c r="C123">
-        <v>0.012173</v>
+        <v>0.001165</v>
       </c>
       <c r="D123">
-        <v>0.001321</v>
+        <v>0.006116</v>
       </c>
       <c r="F123">
-        <v>0.891475</v>
+        <v>-4.248833</v>
       </c>
     </row>
     <row r="124" spans="1:6">
@@ -2494,13 +2494,13 @@
         <v>6</v>
       </c>
       <c r="C124">
-        <v>0.007765</v>
+        <v>0.000675</v>
       </c>
       <c r="D124">
-        <v>0.000543</v>
+        <v>0.00132</v>
       </c>
       <c r="F124">
-        <v>0.930132</v>
+        <v>-0.955976</v>
       </c>
     </row>
     <row r="125" spans="1:6">
@@ -2511,13 +2511,13 @@
         <v>6</v>
       </c>
       <c r="C125">
-        <v>0.003653</v>
+        <v>0.000286</v>
       </c>
       <c r="D125">
-        <v>0.000279</v>
+        <v>0.011211</v>
       </c>
       <c r="F125">
-        <v>0.923588</v>
+        <v>-38.173313</v>
       </c>
     </row>
     <row r="126" spans="1:6">
@@ -2528,13 +2528,13 @@
         <v>6</v>
       </c>
       <c r="C126">
-        <v>0.021063</v>
+        <v>0.002536</v>
       </c>
       <c r="D126">
-        <v>0.005314</v>
+        <v>0.017681</v>
       </c>
       <c r="F126">
-        <v>0.747718</v>
+        <v>-5.972051</v>
       </c>
     </row>
     <row r="127" spans="1:6">
@@ -2545,13 +2545,13 @@
         <v>6</v>
       </c>
       <c r="C127">
-        <v>0.014658</v>
+        <v>0.001629</v>
       </c>
       <c r="D127">
-        <v>0.00229</v>
+        <v>0.00092</v>
       </c>
       <c r="F127">
-        <v>0.843753</v>
+        <v>0.435174</v>
       </c>
     </row>
     <row r="128" spans="1:6">
@@ -2562,13 +2562,13 @@
         <v>6</v>
       </c>
       <c r="C128">
-        <v>0.009572000000000001</v>
+        <v>0.000985</v>
       </c>
       <c r="D128">
-        <v>0.001041</v>
+        <v>0.000567</v>
       </c>
       <c r="F128">
-        <v>0.891271</v>
+        <v>0.424101</v>
       </c>
     </row>
     <row r="129" spans="1:6">
@@ -2579,13 +2579,13 @@
         <v>6</v>
       </c>
       <c r="C129">
-        <v>0.004939</v>
+        <v>0.000455</v>
       </c>
       <c r="D129">
-        <v>0.0005</v>
+        <v>0.005358</v>
       </c>
       <c r="F129">
-        <v>0.898711</v>
+        <v>-10.782079</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
part done whole all data with new model selection
</commit_message>
<xml_diff>
--- a/part2/tables-2/dom_validty_VER_part-2.xlsx
+++ b/part2/tables-2/dom_validty_VER_part-2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="7">
   <si>
     <t>Test ID</t>
   </si>
@@ -420,7 +420,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -429,15 +429,15 @@
         <v>0.001723</v>
       </c>
       <c r="D2">
-        <v>0.014471</v>
+        <v>0.001037</v>
       </c>
       <c r="F2">
-        <v>-7.400321</v>
+        <v>0.39775</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -446,15 +446,15 @@
         <v>0.00079</v>
       </c>
       <c r="D3">
-        <v>0.001747</v>
+        <v>0.000441</v>
       </c>
       <c r="F3">
-        <v>-1.213223</v>
+        <v>0.44164</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -463,15 +463,15 @@
         <v>0.000359</v>
       </c>
       <c r="D4">
-        <v>0.000198</v>
+        <v>0.000189</v>
       </c>
       <c r="F4">
-        <v>0.448397</v>
+        <v>0.47239</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -480,15 +480,15 @@
         <v>0.000188</v>
       </c>
       <c r="D5">
-        <v>3.7E-05</v>
+        <v>0.000114</v>
       </c>
       <c r="F5">
-        <v>0.801739</v>
+        <v>0.39524</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -497,15 +497,15 @@
         <v>0.002414</v>
       </c>
       <c r="D6">
-        <v>0.010186</v>
+        <v>0.001683</v>
       </c>
       <c r="F6">
-        <v>-3.218976</v>
+        <v>0.303132</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -514,15 +514,15 @@
         <v>0.001512</v>
       </c>
       <c r="D7">
-        <v>0.001422</v>
+        <v>0.000902</v>
       </c>
       <c r="F7">
-        <v>0.059733</v>
+        <v>0.403264</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
@@ -531,15 +531,15 @@
         <v>0.000821</v>
       </c>
       <c r="D8">
-        <v>0.000463</v>
+        <v>0.000491</v>
       </c>
       <c r="F8">
-        <v>0.436258</v>
+        <v>0.401818</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
@@ -548,15 +548,15 @@
         <v>0.000418</v>
       </c>
       <c r="D9">
-        <v>4.8E-05</v>
+        <v>0.000196</v>
       </c>
       <c r="F9">
-        <v>0.884895</v>
+        <v>0.531303</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
@@ -565,15 +565,15 @@
         <v>0.000177</v>
       </c>
       <c r="D10">
-        <v>1.8E-05</v>
+        <v>0.000105</v>
       </c>
       <c r="F10">
-        <v>0.900444</v>
+        <v>0.408627</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
@@ -582,15 +582,15 @@
         <v>0.002369</v>
       </c>
       <c r="D11">
-        <v>0.002188</v>
+        <v>0.001967</v>
       </c>
       <c r="F11">
-        <v>0.076156</v>
+        <v>0.169448</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
@@ -599,15 +599,15 @@
         <v>0.001196</v>
       </c>
       <c r="D12">
-        <v>0.000405</v>
+        <v>0.000727</v>
       </c>
       <c r="F12">
-        <v>0.661143</v>
+        <v>0.392092</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
@@ -616,15 +616,15 @@
         <v>0.000583</v>
       </c>
       <c r="D13">
-        <v>7.6E-05</v>
+        <v>0.000316</v>
       </c>
       <c r="F13">
-        <v>0.869185</v>
+        <v>0.458711</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
@@ -633,15 +633,15 @@
         <v>0.000219</v>
       </c>
       <c r="D14">
-        <v>1.6E-05</v>
+        <v>0.000159</v>
       </c>
       <c r="F14">
-        <v>0.924685</v>
+        <v>0.27103</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
         <v>6</v>
@@ -650,15 +650,15 @@
         <v>0.000138</v>
       </c>
       <c r="D15">
-        <v>9E-06</v>
+        <v>0.000109</v>
       </c>
       <c r="F15">
-        <v>0.93346</v>
+        <v>0.203839</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
@@ -667,15 +667,15 @@
         <v>0.001442</v>
       </c>
       <c r="D16">
-        <v>0.000441</v>
+        <v>0.000876</v>
       </c>
       <c r="F16">
-        <v>0.694331</v>
+        <v>0.392114</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
@@ -684,15 +684,15 @@
         <v>0.0009859999999999999</v>
       </c>
       <c r="D17">
-        <v>0.000111</v>
+        <v>0.000425</v>
       </c>
       <c r="F17">
-        <v>0.887834</v>
+        <v>0.5687449999999999</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
@@ -701,15 +701,15 @@
         <v>0.0005330000000000001</v>
       </c>
       <c r="D18">
-        <v>3E-05</v>
+        <v>0.000227</v>
       </c>
       <c r="F18">
-        <v>0.94465</v>
+        <v>0.573429</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
         <v>6</v>
@@ -718,15 +718,15 @@
         <v>0.000253</v>
       </c>
       <c r="D19">
-        <v>1.2E-05</v>
+        <v>0.000145</v>
       </c>
       <c r="F19">
-        <v>0.952387</v>
+        <v>0.427583</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
         <v>6</v>
@@ -735,15 +735,15 @@
         <v>0.002366</v>
       </c>
       <c r="D20">
-        <v>0.000718</v>
+        <v>0.001301</v>
       </c>
       <c r="F20">
-        <v>0.696347</v>
+        <v>0.449906</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B21" t="s">
         <v>6</v>
@@ -752,15 +752,15 @@
         <v>0.001208</v>
       </c>
       <c r="D21">
-        <v>0.000179</v>
+        <v>0.00065</v>
       </c>
       <c r="F21">
-        <v>0.851426</v>
+        <v>0.461529</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
         <v>6</v>
@@ -769,15 +769,15 @@
         <v>0.0007</v>
       </c>
       <c r="D22">
-        <v>5.3E-05</v>
+        <v>0.000342</v>
       </c>
       <c r="F22">
-        <v>0.924806</v>
+        <v>0.5118740000000001</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
         <v>6</v>
@@ -786,15 +786,15 @@
         <v>0.000332</v>
       </c>
       <c r="D23">
-        <v>1.9E-05</v>
+        <v>0.000199</v>
       </c>
       <c r="F23">
-        <v>0.941625</v>
+        <v>0.398926</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
         <v>6</v>
@@ -803,15 +803,15 @@
         <v>0.002846</v>
       </c>
       <c r="D24">
-        <v>0.001122</v>
+        <v>0.001987</v>
       </c>
       <c r="F24">
-        <v>0.605593</v>
+        <v>0.301839</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B25" t="s">
         <v>6</v>
@@ -820,15 +820,15 @@
         <v>0.001858</v>
       </c>
       <c r="D25">
-        <v>0.000369</v>
+        <v>0.001087</v>
       </c>
       <c r="F25">
-        <v>0.801643</v>
+        <v>0.414875</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B26" t="s">
         <v>6</v>
@@ -837,15 +837,15 @@
         <v>0.001024</v>
       </c>
       <c r="D26">
-        <v>0.000132</v>
+        <v>0.000629</v>
       </c>
       <c r="F26">
-        <v>0.870839</v>
+        <v>0.385457</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B27" t="s">
         <v>6</v>
@@ -854,15 +854,15 @@
         <v>0.000489</v>
       </c>
       <c r="D27">
-        <v>5E-05</v>
+        <v>0.000363</v>
       </c>
       <c r="F27">
-        <v>0.898455</v>
+        <v>0.258398</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B28" t="s">
         <v>6</v>
@@ -871,15 +871,15 @@
         <v>0.001752</v>
       </c>
       <c r="D28">
-        <v>0.014471</v>
+        <v>0.001037</v>
       </c>
       <c r="F28">
-        <v>-7.257782</v>
+        <v>0.407969</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B29" t="s">
         <v>6</v>
@@ -888,15 +888,15 @@
         <v>0.000843</v>
       </c>
       <c r="D29">
-        <v>0.001747</v>
+        <v>0.000441</v>
       </c>
       <c r="F29">
-        <v>-1.071954</v>
+        <v>0.47728</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B30" t="s">
         <v>6</v>
@@ -905,15 +905,15 @@
         <v>0.000341</v>
       </c>
       <c r="D30">
-        <v>0.000198</v>
+        <v>0.000189</v>
       </c>
       <c r="F30">
-        <v>0.419366</v>
+        <v>0.444621</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B31" t="s">
         <v>6</v>
@@ -922,15 +922,15 @@
         <v>0.000186</v>
       </c>
       <c r="D31">
-        <v>3.7E-05</v>
+        <v>0.000114</v>
       </c>
       <c r="F31">
-        <v>0.8001</v>
+        <v>0.390242</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B32" t="s">
         <v>6</v>
@@ -939,15 +939,15 @@
         <v>0.002357</v>
       </c>
       <c r="D32">
-        <v>0.010186</v>
+        <v>0.001683</v>
       </c>
       <c r="F32">
-        <v>-3.321883</v>
+        <v>0.286134</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B33" t="s">
         <v>6</v>
@@ -956,15 +956,15 @@
         <v>0.001507</v>
       </c>
       <c r="D33">
-        <v>0.001422</v>
+        <v>0.000902</v>
       </c>
       <c r="F33">
-        <v>0.056291</v>
+        <v>0.401079</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B34" t="s">
         <v>6</v>
@@ -973,15 +973,15 @@
         <v>0.000783</v>
       </c>
       <c r="D34">
-        <v>0.000463</v>
+        <v>0.000491</v>
       </c>
       <c r="F34">
-        <v>0.409113</v>
+        <v>0.373014</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B35" t="s">
         <v>6</v>
@@ -990,15 +990,15 @@
         <v>0.000381</v>
       </c>
       <c r="D35">
-        <v>4.8E-05</v>
+        <v>0.000196</v>
       </c>
       <c r="F35">
-        <v>0.8734960000000001</v>
+        <v>0.484885</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B36" t="s">
         <v>6</v>
@@ -1007,15 +1007,15 @@
         <v>0.000188</v>
       </c>
       <c r="D36">
-        <v>1.8E-05</v>
+        <v>0.000105</v>
       </c>
       <c r="F36">
-        <v>0.906056</v>
+        <v>0.44196</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B37" t="s">
         <v>6</v>
@@ -1024,15 +1024,15 @@
         <v>0.002376</v>
       </c>
       <c r="D37">
-        <v>0.002188</v>
+        <v>0.001967</v>
       </c>
       <c r="F37">
-        <v>0.079211</v>
+        <v>0.172195</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B38" t="s">
         <v>6</v>
@@ -1041,15 +1041,15 @@
         <v>0.00121</v>
       </c>
       <c r="D38">
-        <v>0.000405</v>
+        <v>0.000727</v>
       </c>
       <c r="F38">
-        <v>0.665225</v>
+        <v>0.399416</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B39" t="s">
         <v>6</v>
@@ -1058,15 +1058,15 @@
         <v>0.000583</v>
       </c>
       <c r="D39">
-        <v>7.6E-05</v>
+        <v>0.000316</v>
       </c>
       <c r="F39">
-        <v>0.869185</v>
+        <v>0.458711</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B40" t="s">
         <v>6</v>
@@ -1075,15 +1075,15 @@
         <v>0.000219</v>
       </c>
       <c r="D40">
-        <v>1.6E-05</v>
+        <v>0.000159</v>
       </c>
       <c r="F40">
-        <v>0.924685</v>
+        <v>0.27103</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B41" t="s">
         <v>6</v>
@@ -1092,15 +1092,15 @@
         <v>0.00014</v>
       </c>
       <c r="D41">
-        <v>9E-06</v>
+        <v>0.000109</v>
       </c>
       <c r="F41">
-        <v>0.934648</v>
+        <v>0.218056</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B42" t="s">
         <v>6</v>
@@ -1109,15 +1109,15 @@
         <v>0.001442</v>
       </c>
       <c r="D42">
-        <v>0.000441</v>
+        <v>0.000876</v>
       </c>
       <c r="F42">
-        <v>0.694331</v>
+        <v>0.392114</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B43" t="s">
         <v>6</v>
@@ -1126,15 +1126,15 @@
         <v>0.000973</v>
       </c>
       <c r="D43">
-        <v>0.000111</v>
+        <v>0.000425</v>
       </c>
       <c r="F43">
-        <v>0.886297</v>
+        <v>0.5628379999999999</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B44" t="s">
         <v>6</v>
@@ -1143,15 +1143,15 @@
         <v>0.0005330000000000001</v>
       </c>
       <c r="D44">
-        <v>3E-05</v>
+        <v>0.000227</v>
       </c>
       <c r="F44">
-        <v>0.94465</v>
+        <v>0.573429</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B45" t="s">
         <v>6</v>
@@ -1160,15 +1160,15 @@
         <v>0.00024</v>
       </c>
       <c r="D45">
-        <v>1.2E-05</v>
+        <v>0.000145</v>
       </c>
       <c r="F45">
-        <v>0.949742</v>
+        <v>0.395782</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B46" t="s">
         <v>6</v>
@@ -1177,15 +1177,15 @@
         <v>0.002333</v>
       </c>
       <c r="D46">
-        <v>0.000718</v>
+        <v>0.001301</v>
       </c>
       <c r="F46">
-        <v>0.692045</v>
+        <v>0.442114</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B47" t="s">
         <v>6</v>
@@ -1194,15 +1194,15 @@
         <v>0.00128</v>
       </c>
       <c r="D47">
-        <v>0.000179</v>
+        <v>0.00065</v>
       </c>
       <c r="F47">
-        <v>0.859761</v>
+        <v>0.49174</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B48" t="s">
         <v>6</v>
@@ -1211,15 +1211,15 @@
         <v>0.000675</v>
       </c>
       <c r="D48">
-        <v>5.3E-05</v>
+        <v>0.000342</v>
       </c>
       <c r="F48">
-        <v>0.922072</v>
+        <v>0.494124</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B49" t="s">
         <v>6</v>
@@ -1228,15 +1228,15 @@
         <v>0.000307</v>
       </c>
       <c r="D49">
-        <v>1.9E-05</v>
+        <v>0.000199</v>
       </c>
       <c r="F49">
-        <v>0.936956</v>
+        <v>0.35084</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B50" t="s">
         <v>6</v>
@@ -1245,15 +1245,15 @@
         <v>0.002852</v>
       </c>
       <c r="D50">
-        <v>0.001122</v>
+        <v>0.001987</v>
       </c>
       <c r="F50">
-        <v>0.606442</v>
+        <v>0.303341</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B51" t="s">
         <v>6</v>
@@ -1262,15 +1262,15 @@
         <v>0.001836</v>
       </c>
       <c r="D51">
-        <v>0.000369</v>
+        <v>0.001087</v>
       </c>
       <c r="F51">
-        <v>0.799184</v>
+        <v>0.407621</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B52" t="s">
         <v>6</v>
@@ -1279,15 +1279,15 @@
         <v>0.0009790000000000001</v>
       </c>
       <c r="D52">
-        <v>0.000132</v>
+        <v>0.000629</v>
       </c>
       <c r="F52">
-        <v>0.864832</v>
+        <v>0.356874</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B53" t="s">
         <v>6</v>
@@ -1296,15 +1296,15 @@
         <v>0.000467</v>
       </c>
       <c r="D53">
-        <v>5E-05</v>
+        <v>0.000363</v>
       </c>
       <c r="F53">
-        <v>0.893501</v>
+        <v>0.222222</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B54" t="s">
         <v>6</v>
@@ -1313,15 +1313,15 @@
         <v>0.001937</v>
       </c>
       <c r="D54">
-        <v>0.019933</v>
+        <v>0.001257</v>
       </c>
       <c r="F54">
-        <v>-9.291092000000001</v>
+        <v>0.350864</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B55" t="s">
         <v>6</v>
@@ -1330,15 +1330,15 @@
         <v>0.000802</v>
       </c>
       <c r="D55">
-        <v>0.00254</v>
+        <v>0.000513</v>
       </c>
       <c r="F55">
-        <v>-2.169008</v>
+        <v>0.359405</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B56" t="s">
         <v>6</v>
@@ -1347,15 +1347,15 @@
         <v>0.000353</v>
       </c>
       <c r="D56">
-        <v>0.000282</v>
+        <v>0.000214</v>
       </c>
       <c r="F56">
-        <v>0.200723</v>
+        <v>0.394538</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B57" t="s">
         <v>6</v>
@@ -1364,15 +1364,15 @@
         <v>0.000159</v>
       </c>
       <c r="D57">
-        <v>4.5E-05</v>
+        <v>0.000128</v>
       </c>
       <c r="F57">
-        <v>0.715066</v>
+        <v>0.196475</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B58" t="s">
         <v>6</v>
@@ -1381,15 +1381,15 @@
         <v>0.002717</v>
       </c>
       <c r="D58">
-        <v>0.013792</v>
+        <v>0.00197</v>
       </c>
       <c r="F58">
-        <v>-4.075495</v>
+        <v>0.27488</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B59" t="s">
         <v>6</v>
@@ -1398,15 +1398,15 @@
         <v>0.001656</v>
       </c>
       <c r="D59">
-        <v>0.001982</v>
+        <v>0.001061</v>
       </c>
       <c r="F59">
-        <v>-0.1969</v>
+        <v>0.359632</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B60" t="s">
         <v>6</v>
@@ -1415,15 +1415,15 @@
         <v>0.000879</v>
       </c>
       <c r="D60">
-        <v>0.00061</v>
+        <v>0.000548</v>
       </c>
       <c r="F60">
-        <v>0.306571</v>
+        <v>0.376472</v>
       </c>
     </row>
     <row r="61" spans="1:6">
       <c r="A61">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B61" t="s">
         <v>6</v>
@@ -1432,15 +1432,15 @@
         <v>0.000424</v>
       </c>
       <c r="D61">
-        <v>6.1E-05</v>
+        <v>0.000217</v>
       </c>
       <c r="F61">
-        <v>0.856934</v>
+        <v>0.488518</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B62" t="s">
         <v>6</v>
@@ -1449,15 +1449,15 @@
         <v>0.000165</v>
       </c>
       <c r="D62">
-        <v>2E-05</v>
+        <v>0.000113</v>
       </c>
       <c r="F62">
-        <v>0.880374</v>
+        <v>0.314324</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B63" t="s">
         <v>6</v>
@@ -1466,15 +1466,15 @@
         <v>0.002532</v>
       </c>
       <c r="D63">
-        <v>0.002762</v>
+        <v>0.002226</v>
       </c>
       <c r="F63">
-        <v>-0.091131</v>
+        <v>0.120648</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="A64">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B64" t="s">
         <v>6</v>
@@ -1483,15 +1483,15 @@
         <v>0.001355</v>
       </c>
       <c r="D64">
-        <v>0.000523</v>
+        <v>0.000833</v>
       </c>
       <c r="F64">
-        <v>0.613959</v>
+        <v>0.385717</v>
       </c>
     </row>
     <row r="65" spans="1:6">
       <c r="A65">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B65" t="s">
         <v>6</v>
@@ -1500,15 +1500,15 @@
         <v>0.000603</v>
       </c>
       <c r="D65">
-        <v>9.6E-05</v>
+        <v>0.000352</v>
       </c>
       <c r="F65">
-        <v>0.841245</v>
+        <v>0.415663</v>
       </c>
     </row>
     <row r="66" spans="1:6">
       <c r="A66">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B66" t="s">
         <v>6</v>
@@ -1517,15 +1517,15 @@
         <v>0.000239</v>
       </c>
       <c r="D66">
-        <v>1.9E-05</v>
+        <v>0.000172</v>
       </c>
       <c r="F66">
-        <v>0.918748</v>
+        <v>0.278475</v>
       </c>
     </row>
     <row r="67" spans="1:6">
       <c r="A67">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B67" t="s">
         <v>6</v>
@@ -1534,15 +1534,15 @@
         <v>0.000156</v>
       </c>
       <c r="D67">
-        <v>1E-05</v>
+        <v>0.000124</v>
       </c>
       <c r="F67">
-        <v>0.936098</v>
+        <v>0.208176</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B68" t="s">
         <v>6</v>
@@ -1551,15 +1551,15 @@
         <v>0.001661</v>
       </c>
       <c r="D68">
-        <v>0.000566</v>
+        <v>0.000998</v>
       </c>
       <c r="F68">
-        <v>0.659063</v>
+        <v>0.398827</v>
       </c>
     </row>
     <row r="69" spans="1:6">
       <c r="A69">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B69" t="s">
         <v>6</v>
@@ -1568,15 +1568,15 @@
         <v>0.001039</v>
       </c>
       <c r="D69">
-        <v>0.000138</v>
+        <v>0.000475</v>
       </c>
       <c r="F69">
-        <v>0.867624</v>
+        <v>0.543342</v>
       </c>
     </row>
     <row r="70" spans="1:6">
       <c r="A70">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B70" t="s">
         <v>6</v>
@@ -1585,15 +1585,15 @@
         <v>0.000595</v>
       </c>
       <c r="D70">
-        <v>3.5E-05</v>
+        <v>0.000247</v>
       </c>
       <c r="F70">
-        <v>0.941326</v>
+        <v>0.585468</v>
       </c>
     </row>
     <row r="71" spans="1:6">
       <c r="A71">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B71" t="s">
         <v>6</v>
@@ -1602,15 +1602,15 @@
         <v>0.000307</v>
       </c>
       <c r="D71">
-        <v>1.3E-05</v>
+        <v>0.000157</v>
       </c>
       <c r="F71">
-        <v>0.956219</v>
+        <v>0.489445</v>
       </c>
     </row>
     <row r="72" spans="1:6">
       <c r="A72">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B72" t="s">
         <v>6</v>
@@ -1619,15 +1619,15 @@
         <v>0.002571</v>
       </c>
       <c r="D72">
-        <v>0.000889</v>
+        <v>0.00146</v>
       </c>
       <c r="F72">
-        <v>0.6540859999999999</v>
+        <v>0.432042</v>
       </c>
     </row>
     <row r="73" spans="1:6">
       <c r="A73">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B73" t="s">
         <v>6</v>
@@ -1636,15 +1636,15 @@
         <v>0.001468</v>
       </c>
       <c r="D73">
-        <v>0.00022</v>
+        <v>0.000725</v>
       </c>
       <c r="F73">
-        <v>0.8502150000000001</v>
+        <v>0.505916</v>
       </c>
     </row>
     <row r="74" spans="1:6">
       <c r="A74">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B74" t="s">
         <v>6</v>
@@ -1653,15 +1653,15 @@
         <v>0.0008140000000000001</v>
       </c>
       <c r="D74">
-        <v>6.2E-05</v>
+        <v>0.000376</v>
       </c>
       <c r="F74">
-        <v>0.923565</v>
+        <v>0.5384409999999999</v>
       </c>
     </row>
     <row r="75" spans="1:6">
       <c r="A75">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B75" t="s">
         <v>6</v>
@@ -1670,15 +1670,15 @@
         <v>0.000385</v>
       </c>
       <c r="D75">
-        <v>2.2E-05</v>
+        <v>0.000216</v>
       </c>
       <c r="F75">
-        <v>0.943647</v>
+        <v>0.437566</v>
       </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B76" t="s">
         <v>6</v>
@@ -1687,15 +1687,15 @@
         <v>0.00319</v>
       </c>
       <c r="D76">
-        <v>0.001364</v>
+        <v>0.002203</v>
       </c>
       <c r="F76">
-        <v>0.57229</v>
+        <v>0.309291</v>
       </c>
     </row>
     <row r="77" spans="1:6">
       <c r="A77">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B77" t="s">
         <v>6</v>
@@ -1704,15 +1704,15 @@
         <v>0.002046</v>
       </c>
       <c r="D77">
-        <v>0.000442</v>
+        <v>0.001195</v>
       </c>
       <c r="F77">
-        <v>0.783736</v>
+        <v>0.415713</v>
       </c>
     </row>
     <row r="78" spans="1:6">
       <c r="A78">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B78" t="s">
         <v>6</v>
@@ -1721,15 +1721,15 @@
         <v>0.00119</v>
       </c>
       <c r="D78">
-        <v>0.000155</v>
+        <v>0.000687</v>
       </c>
       <c r="F78">
-        <v>0.869973</v>
+        <v>0.422914</v>
       </c>
     </row>
     <row r="79" spans="1:6">
       <c r="A79">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B79" t="s">
         <v>6</v>
@@ -1738,842 +1738,860 @@
         <v>0.000603</v>
       </c>
       <c r="D79">
-        <v>5.6E-05</v>
+        <v>0.000388</v>
       </c>
       <c r="F79">
-        <v>0.907197</v>
+        <v>0.356376</v>
       </c>
     </row>
     <row r="80" spans="1:6">
       <c r="A80">
-        <v>79</v>
+        <v>81</v>
+      </c>
+      <c r="B80" t="s">
+        <v>6</v>
+      </c>
+      <c r="C80">
+        <v>0.001494</v>
+      </c>
+      <c r="D80">
+        <v>0.001154</v>
       </c>
       <c r="F80">
-        <v>-8.254515</v>
+        <v>0.227399</v>
       </c>
     </row>
     <row r="81" spans="1:6">
       <c r="A81">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B81" t="s">
         <v>6</v>
       </c>
       <c r="C81">
-        <v>0.001494</v>
+        <v>0.000687</v>
       </c>
       <c r="D81">
-        <v>0.013825</v>
+        <v>0.000411</v>
       </c>
       <c r="F81">
-        <v>-1.536155</v>
+        <v>0.401281</v>
       </c>
     </row>
     <row r="82" spans="1:6">
       <c r="A82">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B82" t="s">
         <v>6</v>
       </c>
       <c r="C82">
-        <v>0.000687</v>
+        <v>0.000359</v>
       </c>
       <c r="D82">
-        <v>0.001743</v>
+        <v>0.000222</v>
       </c>
       <c r="F82">
-        <v>0.5338540000000001</v>
+        <v>0.379464</v>
       </c>
     </row>
     <row r="83" spans="1:6">
       <c r="A83">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B83" t="s">
         <v>6</v>
       </c>
       <c r="C83">
-        <v>0.000359</v>
+        <v>0.002438</v>
       </c>
       <c r="D83">
-        <v>0.000167</v>
+        <v>0.0022</v>
       </c>
       <c r="F83">
-        <v>-2.922532</v>
+        <v>0.097279</v>
       </c>
     </row>
     <row r="84" spans="1:6">
       <c r="A84">
-        <v>84</v>
+        <v>86</v>
+      </c>
+      <c r="B84" t="s">
+        <v>6</v>
+      </c>
+      <c r="C84">
+        <v>0.001313</v>
+      </c>
+      <c r="D84">
+        <v>0.000962</v>
       </c>
       <c r="F84">
-        <v>-0.7963519999999999</v>
+        <v>0.267066</v>
       </c>
     </row>
     <row r="85" spans="1:6">
       <c r="A85">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B85" t="s">
         <v>6</v>
       </c>
       <c r="C85">
-        <v>0.002438</v>
+        <v>0.000696</v>
       </c>
       <c r="D85">
-        <v>0.009561999999999999</v>
+        <v>0.000368</v>
       </c>
       <c r="F85">
-        <v>0.686178</v>
+        <v>0.471939</v>
       </c>
     </row>
     <row r="86" spans="1:6">
       <c r="A86">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B86" t="s">
         <v>6</v>
       </c>
       <c r="C86">
-        <v>0.001313</v>
+        <v>0.000348</v>
       </c>
       <c r="D86">
-        <v>0.002358</v>
+        <v>0.000174</v>
       </c>
       <c r="F86">
-        <v>0.878943</v>
+        <v>0.499142</v>
       </c>
     </row>
     <row r="87" spans="1:6">
       <c r="A87">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B87" t="s">
         <v>6</v>
       </c>
       <c r="C87">
-        <v>0.000696</v>
+        <v>0.003559</v>
       </c>
       <c r="D87">
-        <v>0.000219</v>
+        <v>0.003957</v>
       </c>
       <c r="F87">
-        <v>-1.304083</v>
+        <v>-0.111908</v>
       </c>
     </row>
     <row r="88" spans="1:6">
       <c r="A88">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B88" t="s">
         <v>6</v>
       </c>
       <c r="C88">
-        <v>0.000348</v>
+        <v>0.001845</v>
       </c>
       <c r="D88">
-        <v>4.2E-05</v>
+        <v>0.001547</v>
       </c>
       <c r="F88">
-        <v>0.020124</v>
+        <v>0.161384</v>
       </c>
     </row>
     <row r="89" spans="1:6">
       <c r="A89">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B89" t="s">
         <v>6</v>
       </c>
       <c r="C89">
-        <v>0.003559</v>
+        <v>0.000922</v>
       </c>
       <c r="D89">
-        <v>0.008201</v>
+        <v>0.000621</v>
       </c>
       <c r="F89">
-        <v>0.667368</v>
+        <v>0.326979</v>
       </c>
     </row>
     <row r="90" spans="1:6">
       <c r="A90">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B90" t="s">
         <v>6</v>
       </c>
       <c r="C90">
-        <v>0.001845</v>
+        <v>0.000437</v>
       </c>
       <c r="D90">
-        <v>0.001808</v>
+        <v>0.000259</v>
       </c>
       <c r="F90">
-        <v>0.888659</v>
+        <v>0.40822</v>
       </c>
     </row>
     <row r="91" spans="1:6">
       <c r="A91">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B91" t="s">
         <v>6</v>
       </c>
       <c r="C91">
-        <v>0.000922</v>
+        <v>0.000267</v>
       </c>
       <c r="D91">
-        <v>0.000307</v>
+        <v>0.000201</v>
       </c>
       <c r="F91">
-        <v>0.933951</v>
+        <v>0.245922</v>
       </c>
     </row>
     <row r="92" spans="1:6">
       <c r="A92">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B92" t="s">
         <v>6</v>
       </c>
       <c r="C92">
-        <v>0.000437</v>
+        <v>0.002563</v>
       </c>
       <c r="D92">
-        <v>4.9E-05</v>
+        <v>0.001822</v>
       </c>
       <c r="F92">
-        <v>0.259984</v>
+        <v>0.289145</v>
       </c>
     </row>
     <row r="93" spans="1:6">
       <c r="A93">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B93" t="s">
         <v>6</v>
       </c>
       <c r="C93">
-        <v>0.000267</v>
+        <v>0.001443</v>
       </c>
       <c r="D93">
-        <v>1.8E-05</v>
+        <v>0.000834</v>
       </c>
       <c r="F93">
-        <v>0.715278</v>
+        <v>0.421756</v>
       </c>
     </row>
     <row r="94" spans="1:6">
       <c r="A94">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B94" t="s">
         <v>6</v>
       </c>
       <c r="C94">
-        <v>0.002563</v>
+        <v>0.000821</v>
       </c>
       <c r="D94">
-        <v>0.001896</v>
+        <v>0.000394</v>
       </c>
       <c r="F94">
-        <v>0.895151</v>
+        <v>0.520153</v>
       </c>
     </row>
     <row r="95" spans="1:6">
       <c r="A95">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B95" t="s">
         <v>6</v>
       </c>
       <c r="C95">
-        <v>0.001443</v>
+        <v>0.0004</v>
       </c>
       <c r="D95">
-        <v>0.000411</v>
+        <v>0.000218</v>
       </c>
       <c r="F95">
-        <v>0.936978</v>
+        <v>0.455024</v>
       </c>
     </row>
     <row r="96" spans="1:6">
       <c r="A96">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B96" t="s">
         <v>6</v>
       </c>
       <c r="C96">
-        <v>0.000821</v>
+        <v>0.003058</v>
       </c>
       <c r="D96">
-        <v>8.6E-05</v>
+        <v>0.002477</v>
       </c>
       <c r="F96">
-        <v>0.203263</v>
+        <v>0.190004</v>
       </c>
     </row>
     <row r="97" spans="1:6">
       <c r="A97">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B97" t="s">
         <v>6</v>
       </c>
       <c r="C97">
-        <v>0.0004</v>
+        <v>0.001922</v>
       </c>
       <c r="D97">
-        <v>2.5E-05</v>
+        <v>0.00121</v>
       </c>
       <c r="F97">
-        <v>0.690151</v>
+        <v>0.370236</v>
       </c>
     </row>
     <row r="98" spans="1:6">
       <c r="A98">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B98" t="s">
         <v>6</v>
       </c>
       <c r="C98">
-        <v>0.003058</v>
+        <v>0.001104</v>
       </c>
       <c r="D98">
-        <v>0.002437</v>
+        <v>0.0006089999999999999</v>
       </c>
       <c r="F98">
-        <v>0.866038</v>
+        <v>0.448227</v>
       </c>
     </row>
     <row r="99" spans="1:6">
       <c r="A99">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B99" t="s">
         <v>6</v>
       </c>
       <c r="C99">
-        <v>0.001922</v>
+        <v>0.000532</v>
       </c>
       <c r="D99">
-        <v>0.000595</v>
+        <v>0.000312</v>
       </c>
       <c r="F99">
-        <v>0.92228</v>
+        <v>0.413099</v>
       </c>
     </row>
     <row r="100" spans="1:6">
       <c r="A100">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B100" t="s">
         <v>6</v>
       </c>
       <c r="C100">
-        <v>0.001104</v>
+        <v>0.003851</v>
       </c>
       <c r="D100">
-        <v>0.000148</v>
+        <v>0.003533</v>
       </c>
       <c r="F100">
-        <v>0.113569</v>
+        <v>0.08240699999999999</v>
       </c>
     </row>
     <row r="101" spans="1:6">
       <c r="A101">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B101" t="s">
         <v>6</v>
       </c>
       <c r="C101">
-        <v>0.000532</v>
+        <v>0.00258</v>
       </c>
       <c r="D101">
-        <v>4.1E-05</v>
+        <v>0.001917</v>
       </c>
       <c r="F101">
-        <v>0.586824</v>
+        <v>0.256883</v>
       </c>
     </row>
     <row r="102" spans="1:6">
       <c r="A102">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B102" t="s">
         <v>6</v>
       </c>
       <c r="C102">
-        <v>0.003851</v>
+        <v>0.001592</v>
       </c>
       <c r="D102">
-        <v>0.003413</v>
+        <v>0.00104</v>
       </c>
       <c r="F102">
-        <v>0.786783</v>
+        <v>0.346816</v>
       </c>
     </row>
     <row r="103" spans="1:6">
       <c r="A103">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B103" t="s">
         <v>6</v>
       </c>
       <c r="C103">
-        <v>0.00258</v>
+        <v>0.000796</v>
       </c>
       <c r="D103">
-        <v>0.001066</v>
+        <v>0.00055</v>
       </c>
       <c r="F103">
-        <v>0.867309</v>
+        <v>0.308721</v>
       </c>
     </row>
     <row r="104" spans="1:6">
       <c r="A104">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B104" t="s">
         <v>6</v>
       </c>
       <c r="C104">
-        <v>0.001592</v>
+        <v>0.001189</v>
       </c>
       <c r="D104">
-        <v>0.000339</v>
+        <v>0.000498</v>
       </c>
       <c r="F104">
-        <v>-1.777032</v>
+        <v>0.580982</v>
       </c>
     </row>
     <row r="105" spans="1:6">
       <c r="A105">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B105" t="s">
         <v>6</v>
       </c>
       <c r="C105">
-        <v>0.000796</v>
+        <v>0.000478</v>
       </c>
       <c r="D105">
-        <v>0.000106</v>
+        <v>0.00024</v>
       </c>
       <c r="F105">
-        <v>0.251752</v>
+        <v>0.496913</v>
       </c>
     </row>
     <row r="106" spans="1:6">
       <c r="A106">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B106" t="s">
         <v>6</v>
       </c>
       <c r="C106">
-        <v>0.001189</v>
+        <v>0.000209</v>
       </c>
       <c r="D106">
-        <v>0.003302</v>
+        <v>0.00011</v>
       </c>
       <c r="F106">
-        <v>0.719149</v>
+        <v>0.47459</v>
       </c>
     </row>
     <row r="107" spans="1:6">
       <c r="A107">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B107" t="s">
         <v>6</v>
       </c>
       <c r="C107">
-        <v>0.000478</v>
+        <v>9.2E-05</v>
       </c>
       <c r="D107">
-        <v>0.000358</v>
+        <v>6.600000000000001E-05</v>
       </c>
       <c r="F107">
-        <v>0.761657</v>
+        <v>0.279048</v>
       </c>
     </row>
     <row r="108" spans="1:6">
       <c r="A108">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B108" t="s">
         <v>6</v>
       </c>
       <c r="C108">
-        <v>0.000209</v>
+        <v>0.001768</v>
       </c>
       <c r="D108">
-        <v>5.9E-05</v>
+        <v>0.000869</v>
       </c>
       <c r="F108">
-        <v>-0.505393</v>
+        <v>0.508638</v>
       </c>
     </row>
     <row r="109" spans="1:6">
       <c r="A109">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B109" t="s">
         <v>6</v>
       </c>
       <c r="C109">
-        <v>9.2E-05</v>
+        <v>0.001152</v>
       </c>
       <c r="D109">
-        <v>2.2E-05</v>
+        <v>0.00047</v>
       </c>
       <c r="F109">
-        <v>0.691863</v>
+        <v>0.592248</v>
       </c>
     </row>
     <row r="110" spans="1:6">
       <c r="A110">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B110" t="s">
         <v>6</v>
       </c>
       <c r="C110">
-        <v>0.001768</v>
+        <v>0.000589</v>
       </c>
       <c r="D110">
-        <v>0.002661</v>
+        <v>0.000307</v>
       </c>
       <c r="F110">
-        <v>0.733428</v>
+        <v>0.478286</v>
       </c>
     </row>
     <row r="111" spans="1:6">
       <c r="A111">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B111" t="s">
         <v>6</v>
       </c>
       <c r="C111">
-        <v>0.001152</v>
+        <v>0.000316</v>
       </c>
       <c r="D111">
-        <v>0.000355</v>
+        <v>0.00013</v>
       </c>
       <c r="F111">
-        <v>0.931718</v>
+        <v>0.587575</v>
       </c>
     </row>
     <row r="112" spans="1:6">
       <c r="A112">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B112" t="s">
         <v>6</v>
       </c>
       <c r="C112">
-        <v>0.000589</v>
+        <v>0.000124</v>
       </c>
       <c r="D112">
-        <v>0.000157</v>
+        <v>8.1E-05</v>
       </c>
       <c r="F112">
-        <v>0.9039779999999999</v>
+        <v>0.346544</v>
       </c>
     </row>
     <row r="113" spans="1:6">
       <c r="A113">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B113" t="s">
         <v>6</v>
       </c>
       <c r="C113">
-        <v>0.000316</v>
+        <v>0.001918</v>
       </c>
       <c r="D113">
-        <v>2.2E-05</v>
+        <v>0.001149</v>
       </c>
       <c r="F113">
-        <v>0.580817</v>
+        <v>0.401018</v>
       </c>
     </row>
     <row r="114" spans="1:6">
       <c r="A114">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B114" t="s">
         <v>6</v>
       </c>
       <c r="C114">
-        <v>0.000124</v>
+        <v>0.000922</v>
       </c>
       <c r="D114">
-        <v>1.2E-05</v>
+        <v>0.000433</v>
       </c>
       <c r="F114">
-        <v>0.845629</v>
+        <v>0.530342</v>
       </c>
     </row>
     <row r="115" spans="1:6">
       <c r="A115">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B115" t="s">
         <v>6</v>
       </c>
       <c r="C115">
-        <v>0.001918</v>
+        <v>0.000437</v>
       </c>
       <c r="D115">
-        <v>0.000804</v>
+        <v>0.000211</v>
       </c>
       <c r="F115">
-        <v>0.926616</v>
+        <v>0.517091</v>
       </c>
     </row>
     <row r="116" spans="1:6">
       <c r="A116">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B116" t="s">
         <v>6</v>
       </c>
       <c r="C116">
-        <v>0.000922</v>
+        <v>0.000184</v>
       </c>
       <c r="D116">
-        <v>0.000142</v>
+        <v>0.000115</v>
       </c>
       <c r="F116">
-        <v>0.94956</v>
+        <v>0.3752</v>
       </c>
     </row>
     <row r="117" spans="1:6">
       <c r="A117">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B117" t="s">
         <v>6</v>
       </c>
       <c r="C117">
-        <v>0.000437</v>
+        <v>9.7E-05</v>
       </c>
       <c r="D117">
-        <v>3.2E-05</v>
+        <v>7.499999999999999E-05</v>
       </c>
       <c r="F117">
-        <v>0.925277</v>
+        <v>0.231499</v>
       </c>
     </row>
     <row r="118" spans="1:6">
       <c r="A118">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B118" t="s">
         <v>6</v>
       </c>
       <c r="C118">
-        <v>0.000184</v>
+        <v>0.001221</v>
       </c>
       <c r="D118">
-        <v>9E-06</v>
+        <v>0.000506</v>
       </c>
       <c r="F118">
-        <v>0.871974</v>
+        <v>0.58522</v>
       </c>
     </row>
     <row r="119" spans="1:6">
       <c r="A119">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B119" t="s">
         <v>6</v>
       </c>
       <c r="C119">
-        <v>9.7E-05</v>
+        <v>0.000777</v>
       </c>
       <c r="D119">
-        <v>7E-06</v>
+        <v>0.000276</v>
       </c>
       <c r="F119">
-        <v>0.939649</v>
+        <v>0.644262</v>
       </c>
     </row>
     <row r="120" spans="1:6">
       <c r="A120">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B120" t="s">
         <v>6</v>
       </c>
       <c r="C120">
-        <v>0.001221</v>
+        <v>0.000466</v>
       </c>
       <c r="D120">
-        <v>0.000156</v>
+        <v>0.000169</v>
       </c>
       <c r="F120">
-        <v>0.966133</v>
+        <v>0.638401</v>
       </c>
     </row>
     <row r="121" spans="1:6">
       <c r="A121">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B121" t="s">
         <v>6</v>
       </c>
       <c r="C121">
-        <v>0.000777</v>
+        <v>0.0002</v>
       </c>
       <c r="D121">
-        <v>4.7E-05</v>
+        <v>0.000101</v>
       </c>
       <c r="F121">
-        <v>0.95792</v>
+        <v>0.495614</v>
       </c>
     </row>
     <row r="122" spans="1:6">
       <c r="A122">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B122" t="s">
         <v>6</v>
       </c>
       <c r="C122">
-        <v>0.000466</v>
+        <v>0.001881</v>
       </c>
       <c r="D122">
-        <v>1.6E-05</v>
+        <v>0.000782</v>
       </c>
       <c r="F122">
-        <v>0.8451379999999999</v>
+        <v>0.584423</v>
       </c>
     </row>
     <row r="123" spans="1:6">
       <c r="A123">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B123" t="s">
         <v>6</v>
       </c>
       <c r="C123">
-        <v>0.0002</v>
+        <v>0.001165</v>
       </c>
       <c r="D123">
-        <v>8E-06</v>
+        <v>0.000408</v>
       </c>
       <c r="F123">
-        <v>0.932462</v>
+        <v>0.649432</v>
       </c>
     </row>
     <row r="124" spans="1:6">
       <c r="A124">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B124" t="s">
         <v>6</v>
       </c>
       <c r="C124">
-        <v>0.001881</v>
+        <v>0.000675</v>
       </c>
       <c r="D124">
-        <v>0.000291</v>
+        <v>0.000242</v>
       </c>
       <c r="F124">
-        <v>0.958947</v>
+        <v>0.640969</v>
       </c>
     </row>
     <row r="125" spans="1:6">
       <c r="A125">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B125" t="s">
         <v>6</v>
       </c>
       <c r="C125">
-        <v>0.001165</v>
+        <v>0.000286</v>
       </c>
       <c r="D125">
-        <v>7.9E-05</v>
+        <v>0.000133</v>
       </c>
       <c r="F125">
-        <v>0.954273</v>
+        <v>0.536548</v>
       </c>
     </row>
     <row r="126" spans="1:6">
       <c r="A126">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B126" t="s">
         <v>6</v>
       </c>
       <c r="C126">
-        <v>0.000675</v>
+        <v>0.002536</v>
       </c>
       <c r="D126">
-        <v>2.8E-05</v>
+        <v>0.001255</v>
       </c>
       <c r="F126">
-        <v>0.807721</v>
+        <v>0.5049709999999999</v>
       </c>
     </row>
     <row r="127" spans="1:6">
       <c r="A127">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B127" t="s">
         <v>6</v>
       </c>
       <c r="C127">
-        <v>0.000286</v>
+        <v>0.001629</v>
       </c>
       <c r="D127">
-        <v>1.3E-05</v>
+        <v>0.00073</v>
       </c>
       <c r="F127">
-        <v>0.893802</v>
+        <v>0.552084</v>
       </c>
     </row>
     <row r="128" spans="1:6">
       <c r="A128">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B128" t="s">
         <v>6</v>
       </c>
       <c r="C128">
-        <v>0.002536</v>
+        <v>0.000985</v>
       </c>
       <c r="D128">
-        <v>0.000488</v>
+        <v>0.00044</v>
       </c>
       <c r="F128">
-        <v>0.928021</v>
+        <v>0.55361</v>
       </c>
     </row>
     <row r="129" spans="1:6">
       <c r="A129">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B129" t="s">
         <v>6</v>
       </c>
       <c r="C129">
-        <v>0.001629</v>
+        <v>0.000455</v>
       </c>
       <c r="D129">
-        <v>0.000173</v>
+        <v>0.00025</v>
       </c>
       <c r="F129">
-        <v>0.92935</v>
+        <v>0.449825</v>
       </c>
     </row>
   </sheetData>

</xml_diff>